<commit_message>
updated points, smaller icons
</commit_message>
<xml_diff>
--- a/src/data/data.xlsx
+++ b/src/data/data.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="429" uniqueCount="424">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="637" uniqueCount="627">
   <si>
     <t>lat</t>
   </si>
@@ -1305,6 +1305,619 @@
   </si>
   <si>
     <t xml:space="preserve">i thought i did terribly on a quiz i studied so much for. i was mentally drained and didn't want to go back to my unwelcoming complex. i wanted comfort and felt overwhelmed. </t>
+  </si>
+  <si>
+    <t>LatLng(37.87123, -122.25951)</t>
+  </si>
+  <si>
+    <t>I cried here one summer afternoon because I was extremely stressed about failing research and bad grades and not getting into grad school.</t>
+  </si>
+  <si>
+    <t>LatLng(37.8718, -122.26013)</t>
+  </si>
+  <si>
+    <t>I rejected someone's confession, then they came back a few months later and told me I was directly responsible for their crippling depression.  I couldn't handle it and I cried on my way home.</t>
+  </si>
+  <si>
+    <t>LatLng(37.86585, -122.25443)</t>
+  </si>
+  <si>
+    <t>I cried a lot the year I lived in the dorms. Sometimes because of my long-distance relationship, sometimes because of general stress and anxiety, sometimes out of guilt.</t>
+  </si>
+  <si>
+    <t>LatLng(37.87074, -122.25492)</t>
+  </si>
+  <si>
+    <t>Studio all-nighters, sometimes several in a row. Need I say more?</t>
+  </si>
+  <si>
+    <t>LatLng(37.87297, -122.26011)</t>
+  </si>
+  <si>
+    <t>got an F on a midterm, went to some random small path of trees off of memorial glade and called my mom and cried</t>
+  </si>
+  <si>
+    <t>LatLng(37.86762, -122.26431)</t>
+  </si>
+  <si>
+    <t>I had my fingertip cut off during a skateboarding accident first month into college. That's when I came closest to crying, at tang.</t>
+  </si>
+  <si>
+    <t>LatLng(37.8666, -122.25957)</t>
+  </si>
+  <si>
+    <t>finals week and friends being mad at me :(</t>
+  </si>
+  <si>
+    <t>LatLng(37.86953, -122.26401)</t>
+  </si>
+  <si>
+    <t>sad alone and dejected</t>
+  </si>
+  <si>
+    <t>LatLng(37.8735, -122.25878)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I cried in the Hearst concert hall from stress. I didn't feel prepared for my first semester, knew I was severely ill-prepared for Physics 7A. I blamed myself for not studying more, blamed my high school for not having the budget for AP Physics, blamed the fact that growing up poor maybe did affect how I did in college. </t>
+  </si>
+  <si>
+    <t>LatLng(37.87136, -122.25981)</t>
+  </si>
+  <si>
+    <t>Burst out crying when I learned my advisor had terminal cancer. I couldn't stop crying all day, even though I had meetings all over campus -- cried in front of 3 other professors, bursting into tears midway in the conversation and leaving. Literally never talked about it again but I had a little bit of a reputation as being 'unstable' for about a year.</t>
+  </si>
+  <si>
+    <t>LatLng(37.87571, -122.25937)</t>
+  </si>
+  <si>
+    <t>The one time I had test anxiety was in Etch. Had to calm myself down and keep myself from crying all the way right in the middle of the Mech E. computer lab.</t>
+  </si>
+  <si>
+    <t>LatLng(37.87135, -122.2681)</t>
+  </si>
+  <si>
+    <t>I was on my way home from an out-of-town job interview for a job that I knew I didn't get, but more importantly had just realized I didn't want. I felt like I had no idea what I wanted to do after I graduated because I didn't like anything I had done so far and nothing sounded even remotely exciting, not to mention that even if I did figure out what I wanted to do, who would even hire me? I felt just really overwhelmed and lost with no direction so I cried in an uberpool and hoped no one really noticed me.</t>
+  </si>
+  <si>
+    <t>LatLng(37.8674, -122.26325)</t>
+  </si>
+  <si>
+    <t>feeling incredibly alone and distant from the people I used to call my closest friends here</t>
+  </si>
+  <si>
+    <t>LatLng(37.86916, -122.25968)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In my freshman year I was struggling with eating disorder and a general sadness that comes when you're separated from your long-time friends. I felt like I couldn't confide in anyone that I had met, given that we only knew each other for a few months, so I was so lonely. </t>
+  </si>
+  <si>
+    <t>LatLng(37.87008, -122.25525)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I fought with the other leaders of my student organization over ideological and procedural disagreements and gradually came to understand that they wanted me out. I got through our conversation, but barely. Had to find a hallway in Hearst Gym to cry my fucking eyes out. Another friend found me there and I wanted to die of shame. </t>
+  </si>
+  <si>
+    <t>LatLng(37.86577, -122.25423)</t>
+  </si>
+  <si>
+    <t>I had and still am dealing with depression and self-harm. It was late that night and I was walking home alone because all my friends had crashed early. My phone died on me that night so I couldn't get a ride home. I walked home and I was  raped. The scrapes, bruises, and scars are still there and I'll never forget it. I broke down thinking about it and cried, hoping for someone to help.</t>
+  </si>
+  <si>
+    <t>LatLng(37.87556, -122.25869)</t>
+  </si>
+  <si>
+    <t>My parents got divorced a year and a half ago because my father had been cheating on my mother for my whole life, and my mother finally couldn't forgive him any more. He was in town for a meeting. I spoke to him in person for the first time in months. And he was still as selfish as ever. He still dared to make empty promises.  He still thought he was in the right. Afterwards, I hid in the restroom and cried for the loss of the family I thought I had.</t>
+  </si>
+  <si>
+    <t>LatLng(37.86713, -122.26083)</t>
+  </si>
+  <si>
+    <t>I spent my senior year depressed and my long distance boyfriend was at an equally shitty juncture of his life. We broke up over and over and finally we said we were done over spring break. He told me we could still be friends and begged me to stay in touch. I called him a week later when my dog died and he asked what I wanted and why I was calling. He killed every last bit of hope.</t>
+  </si>
+  <si>
+    <t>LatLng(37.86726, -122.2644)</t>
+  </si>
+  <si>
+    <t>I cried because I got a bad midterm grade</t>
+  </si>
+  <si>
+    <t>LatLng(37.87288, -122.26225)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">During my sophomore year a professor and I had a customary meeting about my direction regarding the final assignment. Feeling like I had finally found clarity  — I went to the professor with my idea. He did not agree with my idea and chose to belittle me and disregard my agency. I will always remember him telling me "you clearly lack any form of comprehensive direction, I'm going to have to tell you how it is so sit here and listen." He continued to mansplain to me as I held back tears, I sat on the bench outside and cried. I liked that the bench was situated in such a way that I was the only one on the hill, everyone else below.  </t>
+  </si>
+  <si>
+    <t>LatLng(37.86939, -122.2598)</t>
+  </si>
+  <si>
+    <t>Spring semester of my freshman year I got into a fight with the person I was dating at the time. I went to the steps leading down to Lower Sproul, found a bench to lie down on, and started ugly crying. A few minutes later, while I was still on the phone with my partner, a woman with a kind face approached me and handed me a little sheet of paper. I'm not exaggerating when I say that this was my ugliest cry of all time, like my nose was running, my face was covered in tears, the whole nine yards. I assumed that it was a tissue and i ripped a piece off and blew my nose into it. It was only when the woman looked horrified that I looked down and realized that it was a flyer and that she was trying to invite me to a gathering for her Bible study group. I felt terrible and tried to make an excuse but the situation was funny enough that I finally stopped crying. Months later I passed by the same place again and the same woman was there. She recognized me and tried to invite me to her Bible study group again.</t>
+  </si>
+  <si>
+    <t>LatLng(37.87292, -122.25561)</t>
+  </si>
+  <si>
+    <t>My grandfather died, someone who abused me in the past tried to get in touch with me again, and my depressive disorder was skyrocketing.  I was so out of it that I mixed up a date and missed a midterm.  Broke down sobbing as soon as I realized.</t>
+  </si>
+  <si>
+    <t>LatLng(37.86562, -122.25361)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">in my bed, due to an existential crisis and crippling loneliness </t>
+  </si>
+  <si>
+    <t>LatLng(37.87519, -122.2606)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Being a Daily Cal news editor is stressful </t>
+  </si>
+  <si>
+    <t>LatLng(37.87334, -122.25773)</t>
+  </si>
+  <si>
+    <t>Had to withdraw my semester for mental health reasons</t>
+  </si>
+  <si>
+    <t>LatLng(37.87383, -122.25663)</t>
+  </si>
+  <si>
+    <t>My boss yells at me all the time, and he was being really mean on a day where I had a paper due and a midterm, and had been up since 5 am</t>
+  </si>
+  <si>
+    <t>LatLng(37.86669, -122.25401)</t>
+  </si>
+  <si>
+    <t>it was a rough game day and i had just finished a hard two weeks of midterms and such. called my best friend which made everything better.</t>
+  </si>
+  <si>
+    <t>LatLng(37.86777, -122.26333)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I felt homesick and lonely and just generally incompetent in comparison to everyone else, socially and academically. </t>
+  </si>
+  <si>
+    <t>LatLng(37.86909, -122.26085)</t>
+  </si>
+  <si>
+    <t>Broke down in front of my acting instructor as I explained why I wasn't doing my best in her class. It was the worst month of my college career and was severely depressed, finding it hard to get out of bed, let alone rehearse.  She was kind but I found over the course of that month that Cal is relatively unforgiving and flippant about mental illness. It pushed me to take a year off from school. I did, am now at a different college.</t>
+  </si>
+  <si>
+    <t>LatLng(37.86596, -122.25202)</t>
+  </si>
+  <si>
+    <t>After finding out I had a UTI, continuing my disagreement with my parents, beginning my three-midterm week, my significant other brought me sunflowers from San Francisco.</t>
+  </si>
+  <si>
+    <t>LatLng(37.87504, -122.26017)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I’ve cried at the journalism school because I feel like I’m the least qualified journalist ever. </t>
+  </si>
+  <si>
+    <t>LatLng(37.87596, -122.2579)</t>
+  </si>
+  <si>
+    <t>learned that I could be deeply triggered by a reading assigned for a class; came to terms with the fact that I had been raped.</t>
+  </si>
+  <si>
+    <t>LatLng(37.87547, -122.25546)</t>
+  </si>
+  <si>
+    <t>Turned in my last paper after my last midterm freshman year, and I realised that I would have to go through three more years of sleep deprivation, general anxiety, stress, and feeling inadequate all the time.</t>
+  </si>
+  <si>
+    <t>LatLng(37.86855, -122.25303)</t>
+  </si>
+  <si>
+    <t>Guy I was with abandoned me at a frat party to dance with other girls. I ran out into the street, drunk and alone, and publicly weeped on the streets.</t>
+  </si>
+  <si>
+    <t>LatLng(37.87294, -122.25313)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The boy I loved kissed me (finally!), but after he left my room I broke down crying because I genuinely believe I'd be bad for him.  He's brilliant and I'm a mess. I told him we'd never work and I haven't heard from him since.  </t>
+  </si>
+  <si>
+    <t>cried to my friends because my hookup and I ended things</t>
+  </si>
+  <si>
+    <t>LatLng(37.8688, -122.26822)</t>
+  </si>
+  <si>
+    <t>Lol, I cry at shattuck cinema so much, sometimes it's just nice to watch a movie &amp; cry in the dark</t>
+  </si>
+  <si>
+    <t>LatLng(37.87255, -122.25689)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I was in my science breadth lab one day and I was struggling so much to barely make it past the first two pages meanwhile it seemed that everyone in my group was just zooming past to the middle of the lab and were so difficult to even get help from. I felt so stupid, desperate, frustrated. Maybe if I hadn't come to Cal from a really shitty school in inner city LA. Maybe if I wasn't so poor I could have an easier time learning.  It was the first time in Cal I was actually on the verge of a mental breakdown over poor performance.  Started tearing up in an empty bench by Evans overlooking the bay. It was almost refreshing as well, in a way. </t>
+  </si>
+  <si>
+    <t>LatLng(37.87018, -122.25972)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A friend and I went to an undocumented student healing circle after September 5th. We both cried in each other's arms. </t>
+  </si>
+  <si>
+    <t>LatLng(37.87243, -122.25843)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I remember crying in VLSB 2050. I had a class in which a law professor was being extremely unsensitive about topics concerning sexual harassment. He did not alow students to leave the classroom on their own accord, and if they did so he would call them out and humiliate them in front of the class. I am a survivor and I could not bear to listen to the lecture since it was very disturbing and provoking. I also felt like I could not leave without being questioned so I sat and cried in an amalgam of horror, sadness, and anger. </t>
+  </si>
+  <si>
+    <t>LatLng(37.86611, -122.2559)</t>
+  </si>
+  <si>
+    <t>Homesickness and fear of the future</t>
+  </si>
+  <si>
+    <t>LatLng(37.86784, -122.25122)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Just go a 5/30 on a project I worked over 40 hours for. </t>
+  </si>
+  <si>
+    <t>LatLng(37.87197, -122.25779)</t>
+  </si>
+  <si>
+    <t>Campanile: really missed home and all my friends from high school, felt so lonely and broken. Walked over here at maybe 11:30pm and cried. Something about big structures that let's me feel like I have the permission to be small, to crumble.</t>
+  </si>
+  <si>
+    <t>Spring 2017 semester I had just started seeing a psychiatrist and was trying out different dosages of antidepressants. The one I was trying was making my memory really bad, and one day I was going to leave a class early to go make up a quiz. I completely forgot and with 5 minutes left for me to get there I was sprinting around LeConte trying to find the room while emailing my GSI. He ended up just leaving before i found the room and I sobbed really hard on one of the bridges connecting the buildings. I didn't have DSP at the time and I had already asked him for a few extensions so i never tried to make up that quiz and I stopped going to that discussion after.</t>
+  </si>
+  <si>
+    <t>LatLng(37.86611, -122.25483)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">It was a Friday night and I was feeling lonely. I told myself I needed to go eat and after that I would probably feel better. As I descended the steps from my building, I saw a guy I had studied with multiple times in my math class. I waved and said hi, and he looked at me for a solid 10 seconds with his girlfriend laughing in the background and then looked away, and didn't even reply. I was already alone, and now I just felt more invisible. I went to the bathroom in the Academic Center and started sobbing. I threw water on my face so I wouldn't be in there for too long. </t>
+  </si>
+  <si>
+    <t>LatLng(37.8681, -122.255)</t>
+  </si>
+  <si>
+    <t>I got an email that I was denied in-state tuition for the semester, despite meeting all of the requirements and living in California for over a year. I wasn't sure how to tell my parents that we would pay twice what we originally thought, so I just cried.</t>
+  </si>
+  <si>
+    <t>LatLng(37.87223, -122.25584)</t>
+  </si>
+  <si>
+    <t>I learned that my wonderful, handsome, incredibly brave, honorable boyfriend would never be coming home from deployment.</t>
+  </si>
+  <si>
+    <t>LatLng(37.87323, -122.25301)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I'd been hoping he'd kiss me for a long time, but when he finally did I realized all at once that there was no way I was genuinely in love with him. I just missed the one I let get away. I cried because of how incredibly unfair I had been to this gentle, sweet new guy. </t>
+  </si>
+  <si>
+    <t>LatLng(37.868, -122.25545)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A combination of boy problems, close friends leaving for college, homesickness, and academic stress caused me to break one day. I'm usually someone who bottles up all their emotions until it gets the best of me. </t>
+  </si>
+  <si>
+    <t>LatLng(37.87288, -122.25715)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">After constant feelings of being worthless, incompetent, and simply not being good enough. I felt as if I am never going to be good at anything. I cried inside one of the stalls in the bathroom. </t>
+  </si>
+  <si>
+    <t>LatLng(37.86906, -122.262)</t>
+  </si>
+  <si>
+    <t>I worry about my future and if I'm going to be happy in that image</t>
+  </si>
+  <si>
+    <t>LatLng(37.86981, -122.25512)</t>
+  </si>
+  <si>
+    <t>Stressed about school. Had never asked for an extension on a paper before and felt so pathetic due to not being able to finish it all on time as a college senior. Broke down for a couple hours in the Music Library.</t>
+  </si>
+  <si>
+    <t>LatLng(37.86573, -122.24643)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kissed a same-sex person for the first time at the Clark Kerr track. Was also my first kiss in the rain. I didn't want to be queer. </t>
+  </si>
+  <si>
+    <t>LatLng(37.86882, -122.25246)</t>
+  </si>
+  <si>
+    <t>bawled uncontrollably on a couch during a frat party for no apparently reason</t>
+  </si>
+  <si>
+    <t>LatLng(37.86493, -122.24895)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">got robbed and woke up with the robber in my dorm room
+</t>
+  </si>
+  <si>
+    <t>LatLng(37.86455, -122.26225)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I'm a first generation student, and I am struggling in school. I told my mother about it, and she said, "I'm sorry for being so stupid." 
+I am on the cusp of failing all my classes. </t>
+  </si>
+  <si>
+    <t>LatLng(37.87057, -122.25395)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sad because stressed/overwhelmed with two midterms coming up the next day </t>
+  </si>
+  <si>
+    <t>LatLng(37.87425, -122.25732)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">After a stressful class on ancient Indian history when the professor told us we'd have to memorize a list of roughly 200 mostly undefined Sanskrit terms for the midterm, I cried in the first floor bathroom of Hearst Mining. I just felt utterly overwhelmed. </t>
+  </si>
+  <si>
+    <t>LatLng(37.86881, -122.25777)</t>
+  </si>
+  <si>
+    <t>I was walking up the hill on Bancroft Way in the pouring rain.  I had no umbrella and I was drenched and cold.  This was after I completely gave up on my finals and my dream major.</t>
+  </si>
+  <si>
+    <t>LatLng(37.87336, -122.25483)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Someone I still love a lot told me they had stopped loving me. </t>
+  </si>
+  <si>
+    <t>LatLng(37.87089, -122.25286)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cried in front of my professor about my mental health issues and how out of control my life felt. I had been skipping class for two weeks. </t>
+  </si>
+  <si>
+    <t>LatLng(37.87001, -122.25797)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Last week after meeting with my GSI I stopped in the stairway and cried. I felt stressed overwhelmed and lonely. My GSI told me that I was doing a great job and that I will be fine. But I didnt feel that way. Taking a moment to cry allowed me to relieve some of my stress and have a moment to truly take in what my GSI had to say. </t>
+  </si>
+  <si>
+    <t>LatLng(37.86777, -122.25161)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Freshman year. Felt lonely and isolated. Someone on my floor made a rape joke that really upset me. I was shocked that even at a prestigious institution, people can be so blatantly ignorant. I cried for about thirty minutes.  I wanted to go home. </t>
+  </si>
+  <si>
+    <t>LatLng(37.86771, -122.252)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">My boyfriend and I were having troubles in our relationship. He doesn't go to berkeley, and this is the place we said bye to each other last time he game to visit. I missed him. </t>
+  </si>
+  <si>
+    <t>LatLng(37.87172, -122.25818)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I cried here when my brother called me on the phone to tell me he missed me. </t>
+  </si>
+  <si>
+    <t>LatLng(37.86778, -122.25187)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">All the failure. All the imposter syndrome. All the sadness. </t>
+  </si>
+  <si>
+    <t>LatLng(37.87258, -122.26753)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I cried—bawled—because not only I had just found out that back home, my family was suddenly homeless from an illegal eviction, but our landlord unlawfully threw away all of our stuff. I was standing in front of my apartment door crying, and asking my Mom 'why? why us?'. I remember seeing my neighbors looking at me with such sad faces. I was devastated to learn that all my belongings back home were gone, and that my family had no place to stay, while I was in the midst of finals season. Knowing that my mom, sibling, and nine year old brother would have to fend for themselves while I was at Berkeley took a huge emotional toll on me, something that I eventually had to seek counseling for.  It was as if my house had burned down, and everything in it was taken with the flames. It was especially hard knowing that this all had happened just twenty minutes away from my Berkeley apartment, because my family home was in Oakland. I took a walk around the block and kept crying for the rest of the day. </t>
+  </si>
+  <si>
+    <t>LatLng(37.8653, -122.24972)</t>
+  </si>
+  <si>
+    <t>my friend had just been raped and the rapist was on campus. every day i would come home very overwhelmed and would just cry.</t>
+  </si>
+  <si>
+    <t>LatLng(37.86933, -122.255)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I've cried just being in public due to my chronic anxiety, depression, and borderline personality disorder when I see triggers of my past -regular people, strangers, my assaulters, and former friends. Cal is a small campus and it's okay to cry in public. </t>
+  </si>
+  <si>
+    <t>LatLng(37.87346, -122.25793)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I started crying in front of an advisor that told me that I couldn't study abroad after I had gone through the entire process of signing up and buying my plane ticket ... later to find out he didn't know what he was talking about/lying </t>
+  </si>
+  <si>
+    <t>LatLng(37.86838, -122.26057)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Working at the call center, I talked to a woman who got so mad at me she told me that my major would be worthless entering the job market and that I would never amount to anything significant </t>
+  </si>
+  <si>
+    <t>LatLng(37.86239, -122.26101)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Broke down during the summer because of stress and feeling inadequate compared to my other friends at other schools who seem to get so much more support than Berkeley students are getting. </t>
+  </si>
+  <si>
+    <t>LatLng(37.86998, -122.25802)</t>
+  </si>
+  <si>
+    <t>Performed a poem about my trauma for the Poetry to the People class.  It was the first time in my life I spoke about an incredible act of violence that happened 7 years ago, and I bore my soul to my small 9 person section. I will always be grateful for my pears and the ta's for holding space and helping me heal</t>
+  </si>
+  <si>
+    <t>LatLng(37.87228, -122.25996)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I cried every day this past summer studying MCAT in the blue cubbies of Moffit 5th floor. </t>
+  </si>
+  <si>
+    <t>LatLng(37.87153, -122.26277)</t>
+  </si>
+  <si>
+    <t>procrastinated on another paper and had so much anxiety i just sobbed for an hour in moffitt</t>
+  </si>
+  <si>
+    <t>LatLng(37.87377, -122.26367)</t>
+  </si>
+  <si>
+    <t>grandma passed away and i was basically drunk and crying for a week</t>
+  </si>
+  <si>
+    <t>LatLng(37.87133, -122.25011)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I got a text from a friend who told me that a boy I went to school with passed away while I was sitting in the student section at a football game. I burst into tears and cried while everyone else was cheering for the team and had to sneak out of the stadium past happy drunk teenagers who gave me weird looks.  </t>
+  </si>
+  <si>
+    <t>LatLng(37.86985, -122.25928)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I cried here in the middle of Sprouling for the elections - I felt like I was going to collapse. I wanted to go  home, I wanted to run away despite how hard I worked to get to the place I was in. Running for Senate is a nightmare. But people saw me crying, some looked at me with pity, they saw weakness, but those who knew me looked at me and told me I was powerful and capable. They held my hand - and I later on, I won. </t>
+  </si>
+  <si>
+    <t>LatLng(37.86952, -122.267)</t>
+  </si>
+  <si>
+    <t>I broke down in front of my neighbor in the middle of spring semester my sophomore year. That semester, I was taking 3 technical classes and was heavily involved with my student org and just couldn't keep it in anymore. I'm thankful for him to this day for just lending me his shoulder to cry on and listening to me vent.</t>
+  </si>
+  <si>
+    <t>LatLng(37.86961, -122.26661)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I cried on the way home from school because my nanny had called me and told me that her daughter who had just escaped from her gambler-boyfriend told her that she wanted to get back together with him and that she couldn't do anything about it to stop her since they both lived in Asia. She came from a very poor background and last time, the husband hand sold off all their furniture to gamble. She had no one else to talk to since no one was home at that time, and as I spoke with her, I cried and felt guilty for being stressed and sad about my grades when there are people like her who have bigger and more important issues bugging them. </t>
+  </si>
+  <si>
+    <t>LatLng(37.86812, -122.25504)</t>
+  </si>
+  <si>
+    <t>Cried in the dorms after failing my first midterm ever at Cal and feeling like a failure. Calling home didn't really help either since my mom told me to "just study harder" and "stop getting distracted" in school.</t>
+  </si>
+  <si>
+    <t>LatLng(37.87147, -122.2617)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I cried here after a break up that took me a long time to get over. I had a hard time focusing on school and felt inadequate for not being able to get over the relationship as quickly as I wanted to and felt really disappointed in myself for letting it affect my ambitions. It took me a long time to find motivation again. I still cry sometimes thinking about what a low point it was! </t>
+  </si>
+  <si>
+    <t>LatLng(37.87224, -122.25431)</t>
+  </si>
+  <si>
+    <t>realized my roommate was more attractive than me</t>
+  </si>
+  <si>
+    <t>LatLng(37.8732, -122.26039)</t>
+  </si>
+  <si>
+    <t>It was my first semester at Cal, and I was waiting for the Night Shuttle back home at about 2am when I broke down. I was struggling in all my classes, I missed my family 8000 miles away, and I had no real friends 3 months into college. So I sat there in the cold, alone at 2 in the morning, and cried my heart out.</t>
+  </si>
+  <si>
+    <t>LatLng(37.87321, -122.26067)</t>
+  </si>
+  <si>
+    <t>I had pulled an all nighter through Sunday night, and I wasn't about to sleep anytime soon. I had so much work to do (as everyone else does, I guess). I had been at Mainstacks until 2am, then I went home to Clark Kerr Campus and worked until 6am. Around 8am, I went back to Moffitt, and when I looked at how many hours of class I had that day (7), I felt overwhelmed by regret and tears started streaming down my face as the day began.</t>
+  </si>
+  <si>
+    <t>LatLng(37.8676, -122.26521)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CW: sexual assault, mental health
+my first semester here, I was struggling and dealing with PTSD and depression from being r*ped multiple times by an abusive partner. I was walking down Bancroft and suddenly felt a panic attack coming on, I started crying and ran to Tang for their emergency drop-in counseling, which was helpful. </t>
+  </si>
+  <si>
+    <t>LatLng(37.87305, -122.26023)</t>
+  </si>
+  <si>
+    <t>my family and I were miscommunicating about a weekend-long trip I wanted to take to San Francisco. I was frustrated by their fears, and scared about mine. I wanted to take care of them but it made it too hard to take care of myself, and it felt hard to both be a human with a family and a student with scholastic responsibilities (I had a midterm the next day).</t>
+  </si>
+  <si>
+    <t>LatLng(37.8696, -122.2615)</t>
+  </si>
+  <si>
+    <t>I cried in the SLC listening to a song that hits very close to my heart as I was studying for a midterm.</t>
+  </si>
+  <si>
+    <t>LatLng(37.86588, -122.25532)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cried after thinking how lonely I was and how different the people at Berkeley are compared to what I had at home. </t>
+  </si>
+  <si>
+    <t>LatLng(37.86936, -122.26013)</t>
+  </si>
+  <si>
+    <t>I had just found out that the Public Health major had been canceled at the time. I was originally a math major and so it took an immense toll on me when I found out what I wanted to do was taken away from me. Three semester in and I decided on a major that UC Berkeley wanted to take away. I had called my boyfriend at the time and he offered no advice or comfort so I hung up and cried and called my mom who was a much better help.</t>
+  </si>
+  <si>
+    <t>LatLng(37.87511, -122.25688)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Realizing that my long distance relationship was failing
+</t>
+  </si>
+  <si>
+    <t>LatLng(37.8706, -122.26211)</t>
+  </si>
+  <si>
+    <t>Finished a midterm that was only a D or so for Bio1B on Halloween. I sat and cried at the stone bench around here while little kids nearby were trick or treating. I had one kind man ask me if I was okay, but I was obviously sobbing. This was the first of many eruptions of feeling inadequate and like an affirmative action waste of time.</t>
+  </si>
+  <si>
+    <t>LatLng(37.87305, -122.26024)</t>
+  </si>
+  <si>
+    <t>I came here after my summer Math1A final, a class my dad forced me to enroll in to "raise my GPA" of 1.98 even though I begged him not to because I hadn't even taken algebra and would be better off in humanities. I thought about how weak I was to submit to his will after I tried sticking up for myself and my future at Cal, only to have no choice in fucking myself over for life. Of course I failed the class, and was dismissed, and I'm typing this now from a community college trying to shoot for readmission in a major I chose for myself that I know I can handle. It makes me want to cry now - painful, painful memories of succumbing to the will of a callous parental figure who wanted to use me as a token of prestige.</t>
+  </si>
+  <si>
+    <t>LatLng(37.87443, -122.25821)</t>
+  </si>
+  <si>
+    <t>Here I spoke to an academic counselor who obviously did not care about my situation and could do nothing for me as I burst into tears telling him I'd have to return to an abusive household that couldn't pay eight thousand dollars right away for tuition the next semester. It was the reason my grades suffered so much in the first place, being berated through any mode of communication my family had for me throughout my entire freshman year. And also not having enough financial aid to close the gap I couldn't afford.</t>
+  </si>
+  <si>
+    <t>LatLng(37.87429, -122.25421)</t>
+  </si>
+  <si>
+    <t>I got yet another phone call from my family denigrating me and my self worth because I wasn't able to be in contact with them all day as I had to, you know, study. I sat in my dorm room finally breaking down, and others noticed what bad shape I was in. I quickly noticed a decline in social invites from the people who had been there. I get it. I was a person with problems that nobody wanted to touch. But I felt so utterly alone and unsupported while living here when my blood relations were treating me so badly and I couldn't do anything about it except make them angrier when I stood up for myself. I had no one.</t>
+  </si>
+  <si>
+    <t>LatLng(37.87238, -122.25968)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I've cried in Moffitt more times than I'd like to admit. The last time I cried there, it was 3am and I was reading a book for a life changing class that I truly loved at Cal. The passage went on to talk about a mother, and I started thinking of my own. I was reminded of how this very course, this very major that I wanted to pursue would make her unhappy. It would not only make her unhappy--but sad. I thought about how I couldn't pursue my dreams because she sacrificed her own and her entire being for me. </t>
+  </si>
+  <si>
+    <t>LatLng(37.87977, -122.25715)</t>
+  </si>
+  <si>
+    <t>I was so far behind in all my classes and everything was totally out of control. I had just bombed a midterm and was anxious about it, so I tried coming to lecture but I didn’t understand a single thing. I felt like I wasn’t meant to be here and everyone at home would know I was a fake, and a failure.</t>
+  </si>
+  <si>
+    <t>LatLng(37.86293, -122.26414)</t>
+  </si>
+  <si>
+    <t>i found out my boyfriend is a liar</t>
+  </si>
+  <si>
+    <t>LatLng(37.87526, -122.26117)</t>
+  </si>
+  <si>
+    <t>editing is hard</t>
+  </si>
+  <si>
+    <t>LatLng(37.86929, -122.26003)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The morning after a rape,  I had nowhere to go. I was a commuting student at the time. I wanted to shower, I left my charger at my abusers on Ellsworth. I was shocked. At the Muliticultural Community Center, an intern saw the desperation in my eyes and happily gave me their charger. I broke down in that space.  I'm haunted by it, but it has open arms. </t>
+  </si>
+  <si>
+    <t>LatLng(37.86564, -122.26893)</t>
+  </si>
+  <si>
+    <t>My dog died</t>
+  </si>
+  <si>
+    <t>LatLng(37.87211, -122.26061)</t>
+  </si>
+  <si>
+    <t>LatLng(37.86405, -122.26401)</t>
+  </si>
+  <si>
+    <t>about to bomb an interview in exactly one hour</t>
   </si>
 </sst>
 </file>
@@ -1333,24 +1946,12 @@
     </font>
     <font/>
   </fonts>
-  <fills count="4">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="lightGray"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFF2CC"/>
-        <bgColor rgb="FFFFF2CC"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF4CCCC"/>
-        <bgColor rgb="FFF4CCCC"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -1362,7 +1963,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="12">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -1399,21 +2000,6 @@
     <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="1" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="1" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="1" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -3418,17 +4004,17 @@
       <c r="E132" s="9"/>
     </row>
     <row r="133">
-      <c r="A133" s="12" t="s">
+      <c r="A133" s="6" t="s">
         <v>232</v>
       </c>
       <c r="B133">
-        <f t="shared" ref="B133:B229" si="2">IFERROR(__xludf.DUMMYFUNCTION("SPLIT(SUBSTITUTE(SUBSTITUTE(A133,""LatLng("",""""), "")"", """"), "","")"),"37.86688")</f>
+        <f t="shared" ref="B133:B333" si="2">IFERROR(__xludf.DUMMYFUNCTION("SPLIT(SUBSTITUTE(SUBSTITUTE(A133,""LatLng("",""""), "")"", """"), "","")"),"37.86688")</f>
         <v>37.86688</v>
       </c>
       <c r="C133">
         <v>-122.25794</v>
       </c>
-      <c r="D133" s="13" t="s">
+      <c r="D133" s="8" t="s">
         <v>233</v>
       </c>
       <c r="E133" s="6"/>
@@ -3873,7 +4459,7 @@
       </c>
     </row>
     <row r="162">
-      <c r="A162" s="14" t="s">
+      <c r="A162" s="6" t="s">
         <v>290</v>
       </c>
       <c r="B162">
@@ -3883,19 +4469,19 @@
       <c r="C162">
         <v>-122.26019</v>
       </c>
-      <c r="D162" s="15" t="s">
+      <c r="D162" s="7" t="s">
         <v>291</v>
       </c>
-      <c r="E162" s="14"/>
-      <c r="F162" s="14"/>
-      <c r="G162" s="14"/>
-      <c r="H162" s="14"/>
-      <c r="I162" s="14"/>
-      <c r="J162" s="14"/>
-      <c r="K162" s="14"/>
+      <c r="E162" s="6"/>
+      <c r="F162" s="6"/>
+      <c r="G162" s="6"/>
+      <c r="H162" s="6"/>
+      <c r="I162" s="6"/>
+      <c r="J162" s="6"/>
+      <c r="K162" s="6"/>
     </row>
     <row r="163">
-      <c r="A163" s="14" t="s">
+      <c r="A163" s="6" t="s">
         <v>292</v>
       </c>
       <c r="B163">
@@ -3905,19 +4491,19 @@
       <c r="C163">
         <v>-122.25337</v>
       </c>
-      <c r="D163" s="15" t="s">
+      <c r="D163" s="7" t="s">
         <v>293</v>
       </c>
-      <c r="E163" s="16"/>
-      <c r="F163" s="16"/>
-      <c r="G163" s="16"/>
-      <c r="H163" s="16"/>
-      <c r="I163" s="16"/>
-      <c r="J163" s="16"/>
-      <c r="K163" s="14"/>
+      <c r="E163" s="9"/>
+      <c r="F163" s="9"/>
+      <c r="G163" s="9"/>
+      <c r="H163" s="9"/>
+      <c r="I163" s="9"/>
+      <c r="J163" s="9"/>
+      <c r="K163" s="6"/>
     </row>
     <row r="164">
-      <c r="A164" s="14" t="s">
+      <c r="A164" s="6" t="s">
         <v>294</v>
       </c>
       <c r="B164">
@@ -3927,19 +4513,19 @@
       <c r="C164">
         <v>-122.27079</v>
       </c>
-      <c r="D164" s="15" t="s">
+      <c r="D164" s="7" t="s">
         <v>295</v>
       </c>
-      <c r="E164" s="16"/>
-      <c r="F164" s="16"/>
-      <c r="G164" s="14"/>
-      <c r="H164" s="14"/>
-      <c r="I164" s="14"/>
-      <c r="J164" s="14"/>
-      <c r="K164" s="14"/>
+      <c r="E164" s="9"/>
+      <c r="F164" s="9"/>
+      <c r="G164" s="6"/>
+      <c r="H164" s="6"/>
+      <c r="I164" s="6"/>
+      <c r="J164" s="6"/>
+      <c r="K164" s="6"/>
     </row>
     <row r="165">
-      <c r="A165" s="14" t="s">
+      <c r="A165" s="6" t="s">
         <v>296</v>
       </c>
       <c r="B165">
@@ -3949,19 +4535,19 @@
       <c r="C165">
         <v>-122.25987</v>
       </c>
-      <c r="D165" s="15" t="s">
+      <c r="D165" s="7" t="s">
         <v>297</v>
       </c>
-      <c r="E165" s="16"/>
-      <c r="F165" s="16"/>
-      <c r="G165" s="14"/>
-      <c r="H165" s="14"/>
-      <c r="I165" s="14"/>
-      <c r="J165" s="14"/>
-      <c r="K165" s="14"/>
+      <c r="E165" s="9"/>
+      <c r="F165" s="9"/>
+      <c r="G165" s="6"/>
+      <c r="H165" s="6"/>
+      <c r="I165" s="6"/>
+      <c r="J165" s="6"/>
+      <c r="K165" s="6"/>
     </row>
     <row r="166">
-      <c r="A166" s="14" t="s">
+      <c r="A166" s="6" t="s">
         <v>298</v>
       </c>
       <c r="B166">
@@ -3971,19 +4557,19 @@
       <c r="C166">
         <v>-122.25475</v>
       </c>
-      <c r="D166" s="15" t="s">
+      <c r="D166" s="7" t="s">
         <v>299</v>
       </c>
-      <c r="E166" s="16"/>
-      <c r="F166" s="16"/>
-      <c r="G166" s="16"/>
-      <c r="H166" s="16"/>
-      <c r="I166" s="16"/>
-      <c r="J166" s="16"/>
-      <c r="K166" s="14"/>
+      <c r="E166" s="9"/>
+      <c r="F166" s="9"/>
+      <c r="G166" s="9"/>
+      <c r="H166" s="9"/>
+      <c r="I166" s="9"/>
+      <c r="J166" s="9"/>
+      <c r="K166" s="6"/>
     </row>
     <row r="167">
-      <c r="A167" s="14" t="s">
+      <c r="A167" s="6" t="s">
         <v>300</v>
       </c>
       <c r="B167">
@@ -3993,19 +4579,19 @@
       <c r="C167">
         <v>-122.26111</v>
       </c>
-      <c r="D167" s="14" t="s">
+      <c r="D167" s="6" t="s">
         <v>301</v>
       </c>
-      <c r="E167" s="16"/>
-      <c r="F167" s="16"/>
-      <c r="G167" s="16"/>
-      <c r="H167" s="14"/>
-      <c r="I167" s="14"/>
-      <c r="J167" s="14"/>
-      <c r="K167" s="14"/>
+      <c r="E167" s="9"/>
+      <c r="F167" s="9"/>
+      <c r="G167" s="9"/>
+      <c r="H167" s="6"/>
+      <c r="I167" s="6"/>
+      <c r="J167" s="6"/>
+      <c r="K167" s="6"/>
     </row>
     <row r="168">
-      <c r="A168" s="14" t="s">
+      <c r="A168" s="6" t="s">
         <v>302</v>
       </c>
       <c r="B168">
@@ -4015,19 +4601,19 @@
       <c r="C168">
         <v>-122.26899</v>
       </c>
-      <c r="D168" s="14" t="s">
+      <c r="D168" s="6" t="s">
         <v>303</v>
       </c>
-      <c r="E168" s="16"/>
-      <c r="F168" s="14"/>
-      <c r="G168" s="14"/>
-      <c r="H168" s="14"/>
-      <c r="I168" s="14"/>
-      <c r="J168" s="14"/>
-      <c r="K168" s="14"/>
+      <c r="E168" s="9"/>
+      <c r="F168" s="6"/>
+      <c r="G168" s="6"/>
+      <c r="H168" s="6"/>
+      <c r="I168" s="6"/>
+      <c r="J168" s="6"/>
+      <c r="K168" s="6"/>
     </row>
     <row r="169">
-      <c r="A169" s="14" t="s">
+      <c r="A169" s="6" t="s">
         <v>304</v>
       </c>
       <c r="B169">
@@ -4037,19 +4623,19 @@
       <c r="C169">
         <v>-122.25929</v>
       </c>
-      <c r="D169" s="15" t="s">
+      <c r="D169" s="7" t="s">
         <v>305</v>
       </c>
-      <c r="E169" s="16"/>
-      <c r="F169" s="16"/>
-      <c r="G169" s="16"/>
-      <c r="H169" s="16"/>
-      <c r="I169" s="16"/>
-      <c r="J169" s="16"/>
-      <c r="K169" s="14"/>
+      <c r="E169" s="9"/>
+      <c r="F169" s="9"/>
+      <c r="G169" s="9"/>
+      <c r="H169" s="9"/>
+      <c r="I169" s="9"/>
+      <c r="J169" s="9"/>
+      <c r="K169" s="6"/>
     </row>
     <row r="170">
-      <c r="A170" s="14" t="s">
+      <c r="A170" s="6" t="s">
         <v>306</v>
       </c>
       <c r="B170">
@@ -4059,19 +4645,19 @@
       <c r="C170">
         <v>-122.25955</v>
       </c>
-      <c r="D170" s="15" t="s">
+      <c r="D170" s="7" t="s">
         <v>307</v>
       </c>
-      <c r="E170" s="16"/>
-      <c r="F170" s="16"/>
-      <c r="G170" s="16"/>
-      <c r="H170" s="16"/>
-      <c r="I170" s="16"/>
-      <c r="J170" s="16"/>
-      <c r="K170" s="14"/>
+      <c r="E170" s="9"/>
+      <c r="F170" s="9"/>
+      <c r="G170" s="9"/>
+      <c r="H170" s="9"/>
+      <c r="I170" s="9"/>
+      <c r="J170" s="9"/>
+      <c r="K170" s="6"/>
     </row>
     <row r="171">
-      <c r="A171" s="14" t="s">
+      <c r="A171" s="6" t="s">
         <v>308</v>
       </c>
       <c r="B171">
@@ -4081,19 +4667,19 @@
       <c r="C171">
         <v>-122.26075</v>
       </c>
-      <c r="D171" s="14" t="s">
+      <c r="D171" s="6" t="s">
         <v>309</v>
       </c>
-      <c r="E171" s="14"/>
-      <c r="F171" s="14"/>
-      <c r="G171" s="14"/>
-      <c r="H171" s="14"/>
-      <c r="I171" s="14"/>
-      <c r="J171" s="14"/>
-      <c r="K171" s="14"/>
+      <c r="E171" s="6"/>
+      <c r="F171" s="6"/>
+      <c r="G171" s="6"/>
+      <c r="H171" s="6"/>
+      <c r="I171" s="6"/>
+      <c r="J171" s="6"/>
+      <c r="K171" s="6"/>
     </row>
     <row r="172">
-      <c r="A172" s="14" t="s">
+      <c r="A172" s="6" t="s">
         <v>310</v>
       </c>
       <c r="B172">
@@ -4103,19 +4689,19 @@
       <c r="C172">
         <v>-122.25909</v>
       </c>
-      <c r="D172" s="15" t="s">
+      <c r="D172" s="7" t="s">
         <v>311</v>
       </c>
-      <c r="E172" s="16"/>
-      <c r="F172" s="16"/>
-      <c r="G172" s="16"/>
-      <c r="H172" s="16"/>
-      <c r="I172" s="16"/>
-      <c r="J172" s="14"/>
-      <c r="K172" s="14"/>
+      <c r="E172" s="9"/>
+      <c r="F172" s="9"/>
+      <c r="G172" s="9"/>
+      <c r="H172" s="9"/>
+      <c r="I172" s="9"/>
+      <c r="J172" s="6"/>
+      <c r="K172" s="6"/>
     </row>
     <row r="173">
-      <c r="A173" s="14" t="s">
+      <c r="A173" s="6" t="s">
         <v>312</v>
       </c>
       <c r="B173">
@@ -4125,19 +4711,19 @@
       <c r="C173">
         <v>-122.25514</v>
       </c>
-      <c r="D173" s="15" t="s">
+      <c r="D173" s="7" t="s">
         <v>313</v>
       </c>
-      <c r="E173" s="16"/>
-      <c r="F173" s="14"/>
-      <c r="G173" s="14"/>
-      <c r="H173" s="14"/>
-      <c r="I173" s="14"/>
-      <c r="J173" s="14"/>
-      <c r="K173" s="14"/>
+      <c r="E173" s="9"/>
+      <c r="F173" s="6"/>
+      <c r="G173" s="6"/>
+      <c r="H173" s="6"/>
+      <c r="I173" s="6"/>
+      <c r="J173" s="6"/>
+      <c r="K173" s="6"/>
     </row>
     <row r="174">
-      <c r="A174" s="14" t="s">
+      <c r="A174" s="6" t="s">
         <v>314</v>
       </c>
       <c r="B174">
@@ -4147,19 +4733,19 @@
       <c r="C174">
         <v>-122.25838</v>
       </c>
-      <c r="D174" s="15" t="s">
+      <c r="D174" s="7" t="s">
         <v>315</v>
       </c>
-      <c r="E174" s="16"/>
-      <c r="F174" s="16"/>
-      <c r="G174" s="16"/>
-      <c r="H174" s="16"/>
-      <c r="I174" s="16"/>
-      <c r="J174" s="14"/>
-      <c r="K174" s="14"/>
+      <c r="E174" s="9"/>
+      <c r="F174" s="9"/>
+      <c r="G174" s="9"/>
+      <c r="H174" s="9"/>
+      <c r="I174" s="9"/>
+      <c r="J174" s="6"/>
+      <c r="K174" s="6"/>
     </row>
     <row r="175">
-      <c r="A175" s="14" t="s">
+      <c r="A175" s="6" t="s">
         <v>316</v>
       </c>
       <c r="B175">
@@ -4169,16 +4755,16 @@
       <c r="C175">
         <v>-122.25796</v>
       </c>
-      <c r="D175" s="15" t="s">
+      <c r="D175" s="7" t="s">
         <v>317</v>
       </c>
-      <c r="E175" s="16"/>
-      <c r="F175" s="16"/>
-      <c r="G175" s="16"/>
-      <c r="H175" s="16"/>
-      <c r="I175" s="16"/>
-      <c r="J175" s="16"/>
-      <c r="K175" s="14"/>
+      <c r="E175" s="9"/>
+      <c r="F175" s="9"/>
+      <c r="G175" s="9"/>
+      <c r="H175" s="9"/>
+      <c r="I175" s="9"/>
+      <c r="J175" s="9"/>
+      <c r="K175" s="6"/>
     </row>
     <row r="176">
       <c r="A176" s="6" t="s">
@@ -4211,7 +4797,7 @@
       </c>
     </row>
     <row r="178">
-      <c r="A178" s="12" t="s">
+      <c r="A178" s="6" t="s">
         <v>322</v>
       </c>
       <c r="B178">
@@ -4221,7 +4807,7 @@
       <c r="C178">
         <v>-122.26552</v>
       </c>
-      <c r="D178" s="13" t="s">
+      <c r="D178" s="8" t="s">
         <v>323</v>
       </c>
     </row>
@@ -4301,7 +4887,7 @@
       </c>
     </row>
     <row r="184">
-      <c r="A184" s="14" t="s">
+      <c r="A184" s="6" t="s">
         <v>334</v>
       </c>
       <c r="B184">
@@ -4311,7 +4897,7 @@
       <c r="C184">
         <v>-122.25968</v>
       </c>
-      <c r="D184" s="15" t="s">
+      <c r="D184" s="7" t="s">
         <v>335</v>
       </c>
     </row>
@@ -4988,6 +5574,1566 @@
       </c>
       <c r="D229" s="7" t="s">
         <v>423</v>
+      </c>
+    </row>
+    <row r="230">
+      <c r="A230" s="6" t="s">
+        <v>424</v>
+      </c>
+      <c r="B230">
+        <f t="shared" si="2"/>
+        <v>37.87123</v>
+      </c>
+      <c r="C230">
+        <v>-122.25951</v>
+      </c>
+      <c r="D230" s="7" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="231">
+      <c r="A231" s="6" t="s">
+        <v>424</v>
+      </c>
+      <c r="B231">
+        <f t="shared" si="2"/>
+        <v>37.87123</v>
+      </c>
+      <c r="C231">
+        <v>-122.25951</v>
+      </c>
+      <c r="D231" s="7" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="232">
+      <c r="A232" s="6" t="s">
+        <v>426</v>
+      </c>
+      <c r="B232">
+        <f t="shared" si="2"/>
+        <v>37.8718</v>
+      </c>
+      <c r="C232">
+        <v>-122.26013</v>
+      </c>
+      <c r="D232" s="7" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="233">
+      <c r="A233" s="6" t="s">
+        <v>428</v>
+      </c>
+      <c r="B233">
+        <f t="shared" si="2"/>
+        <v>37.86585</v>
+      </c>
+      <c r="C233">
+        <v>-122.25443</v>
+      </c>
+      <c r="D233" s="7" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="234">
+      <c r="A234" s="6" t="s">
+        <v>430</v>
+      </c>
+      <c r="B234">
+        <f t="shared" si="2"/>
+        <v>37.87074</v>
+      </c>
+      <c r="C234">
+        <v>-122.25492</v>
+      </c>
+      <c r="D234" s="7" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="235">
+      <c r="A235" s="6" t="s">
+        <v>432</v>
+      </c>
+      <c r="B235">
+        <f t="shared" si="2"/>
+        <v>37.87297</v>
+      </c>
+      <c r="C235">
+        <v>-122.26011</v>
+      </c>
+      <c r="D235" s="7" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="236">
+      <c r="A236" s="6" t="s">
+        <v>434</v>
+      </c>
+      <c r="B236">
+        <f t="shared" si="2"/>
+        <v>37.86762</v>
+      </c>
+      <c r="C236">
+        <v>-122.26431</v>
+      </c>
+      <c r="D236" s="7" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="237">
+      <c r="A237" s="6" t="s">
+        <v>436</v>
+      </c>
+      <c r="B237">
+        <f t="shared" si="2"/>
+        <v>37.8666</v>
+      </c>
+      <c r="C237">
+        <v>-122.25957</v>
+      </c>
+      <c r="D237" s="7" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="238">
+      <c r="A238" s="6" t="s">
+        <v>438</v>
+      </c>
+      <c r="B238">
+        <f t="shared" si="2"/>
+        <v>37.86953</v>
+      </c>
+      <c r="C238">
+        <v>-122.26401</v>
+      </c>
+      <c r="D238" s="10" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="239">
+      <c r="A239" s="6" t="s">
+        <v>440</v>
+      </c>
+      <c r="B239">
+        <f t="shared" si="2"/>
+        <v>37.8735</v>
+      </c>
+      <c r="C239">
+        <v>-122.25878</v>
+      </c>
+      <c r="D239" s="7" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="240">
+      <c r="A240" s="6" t="s">
+        <v>442</v>
+      </c>
+      <c r="B240">
+        <f t="shared" si="2"/>
+        <v>37.87136</v>
+      </c>
+      <c r="C240">
+        <v>-122.25981</v>
+      </c>
+      <c r="D240" s="7" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="241">
+      <c r="A241" s="6" t="s">
+        <v>444</v>
+      </c>
+      <c r="B241">
+        <f t="shared" si="2"/>
+        <v>37.87571</v>
+      </c>
+      <c r="C241">
+        <v>-122.25937</v>
+      </c>
+      <c r="D241" s="7" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="242">
+      <c r="A242" s="6" t="s">
+        <v>446</v>
+      </c>
+      <c r="B242">
+        <f t="shared" si="2"/>
+        <v>37.87135</v>
+      </c>
+      <c r="C242">
+        <v>-122.2681</v>
+      </c>
+      <c r="D242" s="7" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="243">
+      <c r="A243" s="6" t="s">
+        <v>448</v>
+      </c>
+      <c r="B243">
+        <f t="shared" si="2"/>
+        <v>37.8674</v>
+      </c>
+      <c r="C243">
+        <v>-122.26325</v>
+      </c>
+      <c r="D243" s="7" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="244">
+      <c r="A244" s="6" t="s">
+        <v>450</v>
+      </c>
+      <c r="B244">
+        <f t="shared" si="2"/>
+        <v>37.86916</v>
+      </c>
+      <c r="C244">
+        <v>-122.25968</v>
+      </c>
+      <c r="D244" s="7" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="245">
+      <c r="A245" s="6" t="s">
+        <v>452</v>
+      </c>
+      <c r="B245">
+        <f t="shared" si="2"/>
+        <v>37.87008</v>
+      </c>
+      <c r="C245">
+        <v>-122.25525</v>
+      </c>
+      <c r="D245" s="7" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="246">
+      <c r="A246" s="6" t="s">
+        <v>454</v>
+      </c>
+      <c r="B246">
+        <f t="shared" si="2"/>
+        <v>37.86577</v>
+      </c>
+      <c r="C246">
+        <v>-122.25423</v>
+      </c>
+      <c r="D246" s="7" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="247">
+      <c r="A247" s="6" t="s">
+        <v>456</v>
+      </c>
+      <c r="B247">
+        <f t="shared" si="2"/>
+        <v>37.87556</v>
+      </c>
+      <c r="C247">
+        <v>-122.25869</v>
+      </c>
+      <c r="D247" s="7" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="248">
+      <c r="A248" s="6" t="s">
+        <v>458</v>
+      </c>
+      <c r="B248">
+        <f t="shared" si="2"/>
+        <v>37.86713</v>
+      </c>
+      <c r="C248">
+        <v>-122.26083</v>
+      </c>
+      <c r="D248" s="7" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="249">
+      <c r="A249" s="6" t="s">
+        <v>460</v>
+      </c>
+      <c r="B249">
+        <f t="shared" si="2"/>
+        <v>37.86726</v>
+      </c>
+      <c r="C249">
+        <v>-122.2644</v>
+      </c>
+      <c r="D249" s="7" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="250">
+      <c r="A250" s="6" t="s">
+        <v>462</v>
+      </c>
+      <c r="B250">
+        <f t="shared" si="2"/>
+        <v>37.87288</v>
+      </c>
+      <c r="C250">
+        <v>-122.26225</v>
+      </c>
+      <c r="D250" s="6" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="251">
+      <c r="A251" s="6" t="s">
+        <v>464</v>
+      </c>
+      <c r="B251">
+        <f t="shared" si="2"/>
+        <v>37.86939</v>
+      </c>
+      <c r="C251">
+        <v>-122.2598</v>
+      </c>
+      <c r="D251" s="6" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="252">
+      <c r="A252" s="6" t="s">
+        <v>466</v>
+      </c>
+      <c r="B252">
+        <f t="shared" si="2"/>
+        <v>37.87292</v>
+      </c>
+      <c r="C252">
+        <v>-122.25561</v>
+      </c>
+      <c r="D252" s="7" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="253">
+      <c r="A253" s="6" t="s">
+        <v>468</v>
+      </c>
+      <c r="B253">
+        <f t="shared" si="2"/>
+        <v>37.86562</v>
+      </c>
+      <c r="C253">
+        <v>-122.25361</v>
+      </c>
+      <c r="D253" s="7" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="254">
+      <c r="A254" s="6" t="s">
+        <v>470</v>
+      </c>
+      <c r="B254">
+        <f t="shared" si="2"/>
+        <v>37.87519</v>
+      </c>
+      <c r="C254">
+        <v>-122.2606</v>
+      </c>
+      <c r="D254" s="7" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="255">
+      <c r="A255" s="6" t="s">
+        <v>472</v>
+      </c>
+      <c r="B255">
+        <f t="shared" si="2"/>
+        <v>37.87334</v>
+      </c>
+      <c r="C255">
+        <v>-122.25773</v>
+      </c>
+      <c r="D255" s="7" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="256">
+      <c r="A256" s="6" t="s">
+        <v>474</v>
+      </c>
+      <c r="B256">
+        <f t="shared" si="2"/>
+        <v>37.87383</v>
+      </c>
+      <c r="C256">
+        <v>-122.25663</v>
+      </c>
+      <c r="D256" s="7" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="257">
+      <c r="A257" s="6" t="s">
+        <v>476</v>
+      </c>
+      <c r="B257">
+        <f t="shared" si="2"/>
+        <v>37.86669</v>
+      </c>
+      <c r="C257">
+        <v>-122.25401</v>
+      </c>
+      <c r="D257" s="7" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="258">
+      <c r="A258" s="6" t="s">
+        <v>478</v>
+      </c>
+      <c r="B258">
+        <f t="shared" si="2"/>
+        <v>37.86777</v>
+      </c>
+      <c r="C258">
+        <v>-122.26333</v>
+      </c>
+      <c r="D258" s="7" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="259">
+      <c r="A259" s="6" t="s">
+        <v>480</v>
+      </c>
+      <c r="B259">
+        <f t="shared" si="2"/>
+        <v>37.86909</v>
+      </c>
+      <c r="C259">
+        <v>-122.26085</v>
+      </c>
+      <c r="D259" s="6" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="260">
+      <c r="A260" s="6" t="s">
+        <v>482</v>
+      </c>
+      <c r="B260">
+        <f t="shared" si="2"/>
+        <v>37.86596</v>
+      </c>
+      <c r="C260">
+        <v>-122.25202</v>
+      </c>
+      <c r="D260" s="7" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="261">
+      <c r="A261" s="6" t="s">
+        <v>484</v>
+      </c>
+      <c r="B261">
+        <f t="shared" si="2"/>
+        <v>37.87504</v>
+      </c>
+      <c r="C261">
+        <v>-122.26017</v>
+      </c>
+      <c r="D261" s="7" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="262">
+      <c r="A262" s="6" t="s">
+        <v>486</v>
+      </c>
+      <c r="B262">
+        <f t="shared" si="2"/>
+        <v>37.87596</v>
+      </c>
+      <c r="C262">
+        <v>-122.2579</v>
+      </c>
+      <c r="D262" s="7" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="263">
+      <c r="A263" s="6" t="s">
+        <v>488</v>
+      </c>
+      <c r="B263">
+        <f t="shared" si="2"/>
+        <v>37.87547</v>
+      </c>
+      <c r="C263">
+        <v>-122.25546</v>
+      </c>
+      <c r="D263" s="6" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="264">
+      <c r="A264" s="6" t="s">
+        <v>490</v>
+      </c>
+      <c r="B264">
+        <f t="shared" si="2"/>
+        <v>37.86855</v>
+      </c>
+      <c r="C264">
+        <v>-122.25303</v>
+      </c>
+      <c r="D264" s="8" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="265">
+      <c r="A265" s="6" t="s">
+        <v>492</v>
+      </c>
+      <c r="B265">
+        <f t="shared" si="2"/>
+        <v>37.87294</v>
+      </c>
+      <c r="C265">
+        <v>-122.25313</v>
+      </c>
+      <c r="D265" s="7" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="266">
+      <c r="A266" s="6" t="s">
+        <v>362</v>
+      </c>
+      <c r="B266">
+        <f t="shared" si="2"/>
+        <v>37.87147</v>
+      </c>
+      <c r="C266">
+        <v>-122.26434</v>
+      </c>
+      <c r="D266" s="7" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="267">
+      <c r="A267" s="6" t="s">
+        <v>495</v>
+      </c>
+      <c r="B267">
+        <f t="shared" si="2"/>
+        <v>37.8688</v>
+      </c>
+      <c r="C267">
+        <v>-122.26822</v>
+      </c>
+      <c r="D267" s="7" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="268">
+      <c r="A268" s="6" t="s">
+        <v>497</v>
+      </c>
+      <c r="B268">
+        <f t="shared" si="2"/>
+        <v>37.87255</v>
+      </c>
+      <c r="C268">
+        <v>-122.25689</v>
+      </c>
+      <c r="D268" s="7" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="269">
+      <c r="A269" s="6" t="s">
+        <v>499</v>
+      </c>
+      <c r="B269">
+        <f t="shared" si="2"/>
+        <v>37.87018</v>
+      </c>
+      <c r="C269">
+        <v>-122.25972</v>
+      </c>
+      <c r="D269" s="7" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="270">
+      <c r="A270" s="6" t="s">
+        <v>501</v>
+      </c>
+      <c r="B270">
+        <f t="shared" si="2"/>
+        <v>37.87243</v>
+      </c>
+      <c r="C270">
+        <v>-122.25843</v>
+      </c>
+      <c r="D270" s="7" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="271">
+      <c r="A271" s="6" t="s">
+        <v>503</v>
+      </c>
+      <c r="B271">
+        <f t="shared" si="2"/>
+        <v>37.86611</v>
+      </c>
+      <c r="C271">
+        <v>-122.2559</v>
+      </c>
+      <c r="D271" s="7" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="272">
+      <c r="A272" s="6" t="s">
+        <v>505</v>
+      </c>
+      <c r="B272">
+        <f t="shared" si="2"/>
+        <v>37.86784</v>
+      </c>
+      <c r="C272">
+        <v>-122.25122</v>
+      </c>
+      <c r="D272" s="7" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="273">
+      <c r="A273" s="6" t="s">
+        <v>507</v>
+      </c>
+      <c r="B273">
+        <f t="shared" si="2"/>
+        <v>37.87197</v>
+      </c>
+      <c r="C273">
+        <v>-122.25779</v>
+      </c>
+      <c r="D273" s="7" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="274">
+      <c r="A274" s="6" t="s">
+        <v>242</v>
+      </c>
+      <c r="B274">
+        <f t="shared" si="2"/>
+        <v>37.87148</v>
+      </c>
+      <c r="C274">
+        <v>-122.26466</v>
+      </c>
+      <c r="D274" s="6" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="275">
+      <c r="A275" s="6" t="s">
+        <v>510</v>
+      </c>
+      <c r="B275">
+        <f t="shared" si="2"/>
+        <v>37.86611</v>
+      </c>
+      <c r="C275">
+        <v>-122.25483</v>
+      </c>
+      <c r="D275" s="7" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="276">
+      <c r="A276" s="6" t="s">
+        <v>512</v>
+      </c>
+      <c r="B276">
+        <f t="shared" si="2"/>
+        <v>37.8681</v>
+      </c>
+      <c r="C276">
+        <v>-122.255</v>
+      </c>
+      <c r="D276" s="6" t="s">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="277">
+      <c r="A277" s="6" t="s">
+        <v>514</v>
+      </c>
+      <c r="B277">
+        <f t="shared" si="2"/>
+        <v>37.87223</v>
+      </c>
+      <c r="C277">
+        <v>-122.25584</v>
+      </c>
+      <c r="D277" s="7" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="278">
+      <c r="A278" s="6" t="s">
+        <v>516</v>
+      </c>
+      <c r="B278">
+        <f t="shared" si="2"/>
+        <v>37.87323</v>
+      </c>
+      <c r="C278">
+        <v>-122.25301</v>
+      </c>
+      <c r="D278" s="7" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="279">
+      <c r="A279" s="6" t="s">
+        <v>518</v>
+      </c>
+      <c r="B279">
+        <f t="shared" si="2"/>
+        <v>37.868</v>
+      </c>
+      <c r="C279">
+        <v>-122.25545</v>
+      </c>
+      <c r="D279" s="7" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="280">
+      <c r="A280" s="6" t="s">
+        <v>520</v>
+      </c>
+      <c r="B280">
+        <f t="shared" si="2"/>
+        <v>37.87288</v>
+      </c>
+      <c r="C280">
+        <v>-122.25715</v>
+      </c>
+      <c r="D280" s="7" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="281">
+      <c r="A281" s="6" t="s">
+        <v>522</v>
+      </c>
+      <c r="B281">
+        <f t="shared" si="2"/>
+        <v>37.86906</v>
+      </c>
+      <c r="C281">
+        <v>-122.262</v>
+      </c>
+      <c r="D281" s="7" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="282">
+      <c r="A282" s="6" t="s">
+        <v>524</v>
+      </c>
+      <c r="B282">
+        <f t="shared" si="2"/>
+        <v>37.86981</v>
+      </c>
+      <c r="C282">
+        <v>-122.25512</v>
+      </c>
+      <c r="D282" s="7" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="283">
+      <c r="A283" s="6" t="s">
+        <v>526</v>
+      </c>
+      <c r="B283">
+        <f t="shared" si="2"/>
+        <v>37.86573</v>
+      </c>
+      <c r="C283">
+        <v>-122.24643</v>
+      </c>
+      <c r="D283" s="7" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="284">
+      <c r="A284" s="6" t="s">
+        <v>528</v>
+      </c>
+      <c r="B284">
+        <f t="shared" si="2"/>
+        <v>37.86882</v>
+      </c>
+      <c r="C284">
+        <v>-122.25246</v>
+      </c>
+      <c r="D284" s="7" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="285">
+      <c r="A285" s="6" t="s">
+        <v>530</v>
+      </c>
+      <c r="B285">
+        <f t="shared" si="2"/>
+        <v>37.86493</v>
+      </c>
+      <c r="C285">
+        <v>-122.24895</v>
+      </c>
+      <c r="D285" s="7" t="s">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="286">
+      <c r="A286" s="6" t="s">
+        <v>532</v>
+      </c>
+      <c r="B286">
+        <f t="shared" si="2"/>
+        <v>37.86455</v>
+      </c>
+      <c r="C286">
+        <v>-122.26225</v>
+      </c>
+      <c r="D286" s="7" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="287">
+      <c r="A287" s="6" t="s">
+        <v>534</v>
+      </c>
+      <c r="B287">
+        <f t="shared" si="2"/>
+        <v>37.87057</v>
+      </c>
+      <c r="C287">
+        <v>-122.25395</v>
+      </c>
+      <c r="D287" s="7" t="s">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="288">
+      <c r="A288" s="6" t="s">
+        <v>536</v>
+      </c>
+      <c r="B288">
+        <f t="shared" si="2"/>
+        <v>37.87425</v>
+      </c>
+      <c r="C288">
+        <v>-122.25732</v>
+      </c>
+      <c r="D288" s="6" t="s">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="289">
+      <c r="A289" s="6" t="s">
+        <v>538</v>
+      </c>
+      <c r="B289">
+        <f t="shared" si="2"/>
+        <v>37.86881</v>
+      </c>
+      <c r="C289">
+        <v>-122.25777</v>
+      </c>
+      <c r="D289" s="7" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="290">
+      <c r="A290" s="6" t="s">
+        <v>540</v>
+      </c>
+      <c r="B290">
+        <f t="shared" si="2"/>
+        <v>37.87336</v>
+      </c>
+      <c r="C290">
+        <v>-122.25483</v>
+      </c>
+      <c r="D290" s="7" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="291">
+      <c r="A291" s="6" t="s">
+        <v>542</v>
+      </c>
+      <c r="B291">
+        <f t="shared" si="2"/>
+        <v>37.87089</v>
+      </c>
+      <c r="C291">
+        <v>-122.25286</v>
+      </c>
+      <c r="D291" s="7" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="292">
+      <c r="A292" s="6" t="s">
+        <v>544</v>
+      </c>
+      <c r="B292">
+        <f t="shared" si="2"/>
+        <v>37.87001</v>
+      </c>
+      <c r="C292">
+        <v>-122.25797</v>
+      </c>
+      <c r="D292" s="7" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="293">
+      <c r="A293" s="6" t="s">
+        <v>546</v>
+      </c>
+      <c r="B293">
+        <f t="shared" si="2"/>
+        <v>37.86777</v>
+      </c>
+      <c r="C293">
+        <v>-122.25161</v>
+      </c>
+      <c r="D293" s="7" t="s">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="294">
+      <c r="A294" s="6" t="s">
+        <v>548</v>
+      </c>
+      <c r="B294">
+        <f t="shared" si="2"/>
+        <v>37.86771</v>
+      </c>
+      <c r="C294">
+        <v>-122.252</v>
+      </c>
+      <c r="D294" s="7" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="295">
+      <c r="A295" s="6" t="s">
+        <v>550</v>
+      </c>
+      <c r="B295">
+        <f t="shared" si="2"/>
+        <v>37.87172</v>
+      </c>
+      <c r="C295">
+        <v>-122.25818</v>
+      </c>
+      <c r="D295" s="7" t="s">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="296">
+      <c r="A296" s="6" t="s">
+        <v>552</v>
+      </c>
+      <c r="B296">
+        <f t="shared" si="2"/>
+        <v>37.86778</v>
+      </c>
+      <c r="C296">
+        <v>-122.25187</v>
+      </c>
+      <c r="D296" s="7" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="297">
+      <c r="A297" s="6" t="s">
+        <v>554</v>
+      </c>
+      <c r="B297">
+        <f t="shared" si="2"/>
+        <v>37.87258</v>
+      </c>
+      <c r="C297">
+        <v>-122.26753</v>
+      </c>
+      <c r="D297" s="10" t="s">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="298">
+      <c r="A298" s="6" t="s">
+        <v>556</v>
+      </c>
+      <c r="B298">
+        <f t="shared" si="2"/>
+        <v>37.8653</v>
+      </c>
+      <c r="C298">
+        <v>-122.24972</v>
+      </c>
+      <c r="D298" s="8" t="s">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="299">
+      <c r="A299" s="6" t="s">
+        <v>558</v>
+      </c>
+      <c r="B299">
+        <f t="shared" si="2"/>
+        <v>37.86933</v>
+      </c>
+      <c r="C299">
+        <v>-122.255</v>
+      </c>
+      <c r="D299" s="6" t="s">
+        <v>559</v>
+      </c>
+    </row>
+    <row r="300">
+      <c r="A300" s="6" t="s">
+        <v>560</v>
+      </c>
+      <c r="B300">
+        <f t="shared" si="2"/>
+        <v>37.87346</v>
+      </c>
+      <c r="C300">
+        <v>-122.25793</v>
+      </c>
+      <c r="D300" s="7" t="s">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="301">
+      <c r="A301" s="6" t="s">
+        <v>562</v>
+      </c>
+      <c r="B301">
+        <f t="shared" si="2"/>
+        <v>37.86838</v>
+      </c>
+      <c r="C301">
+        <v>-122.26057</v>
+      </c>
+      <c r="D301" s="7" t="s">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="302">
+      <c r="A302" s="6" t="s">
+        <v>564</v>
+      </c>
+      <c r="B302">
+        <f t="shared" si="2"/>
+        <v>37.86239</v>
+      </c>
+      <c r="C302">
+        <v>-122.26101</v>
+      </c>
+      <c r="D302" s="7" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="303">
+      <c r="A303" s="6" t="s">
+        <v>566</v>
+      </c>
+      <c r="B303">
+        <f t="shared" si="2"/>
+        <v>37.86998</v>
+      </c>
+      <c r="C303">
+        <v>-122.25802</v>
+      </c>
+      <c r="D303" s="6" t="s">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="304">
+      <c r="A304" s="6" t="s">
+        <v>568</v>
+      </c>
+      <c r="B304">
+        <f t="shared" si="2"/>
+        <v>37.87228</v>
+      </c>
+      <c r="C304">
+        <v>-122.25996</v>
+      </c>
+      <c r="D304" s="7" t="s">
+        <v>569</v>
+      </c>
+    </row>
+    <row r="305">
+      <c r="A305" s="6" t="s">
+        <v>570</v>
+      </c>
+      <c r="B305">
+        <f t="shared" si="2"/>
+        <v>37.87153</v>
+      </c>
+      <c r="C305">
+        <v>-122.26277</v>
+      </c>
+      <c r="D305" s="7" t="s">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="306">
+      <c r="A306" s="6" t="s">
+        <v>572</v>
+      </c>
+      <c r="B306">
+        <f t="shared" si="2"/>
+        <v>37.87377</v>
+      </c>
+      <c r="C306">
+        <v>-122.26367</v>
+      </c>
+      <c r="D306" s="7" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="307">
+      <c r="A307" s="6" t="s">
+        <v>574</v>
+      </c>
+      <c r="B307">
+        <f t="shared" si="2"/>
+        <v>37.87133</v>
+      </c>
+      <c r="C307">
+        <v>-122.25011</v>
+      </c>
+      <c r="D307" s="10" t="s">
+        <v>575</v>
+      </c>
+    </row>
+    <row r="308">
+      <c r="A308" s="6" t="s">
+        <v>576</v>
+      </c>
+      <c r="B308">
+        <f t="shared" si="2"/>
+        <v>37.86985</v>
+      </c>
+      <c r="C308">
+        <v>-122.25928</v>
+      </c>
+      <c r="D308" s="7" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="309">
+      <c r="A309" s="6" t="s">
+        <v>578</v>
+      </c>
+      <c r="B309">
+        <f t="shared" si="2"/>
+        <v>37.86952</v>
+      </c>
+      <c r="C309">
+        <v>-122.267</v>
+      </c>
+      <c r="D309" s="7" t="s">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="310">
+      <c r="A310" s="6" t="s">
+        <v>580</v>
+      </c>
+      <c r="B310">
+        <f t="shared" si="2"/>
+        <v>37.86961</v>
+      </c>
+      <c r="C310">
+        <v>-122.26661</v>
+      </c>
+      <c r="D310" s="7" t="s">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="311">
+      <c r="A311" s="6" t="s">
+        <v>582</v>
+      </c>
+      <c r="B311">
+        <f t="shared" si="2"/>
+        <v>37.86812</v>
+      </c>
+      <c r="C311">
+        <v>-122.25504</v>
+      </c>
+      <c r="D311" s="7" t="s">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="312">
+      <c r="A312" s="6" t="s">
+        <v>584</v>
+      </c>
+      <c r="B312">
+        <f t="shared" si="2"/>
+        <v>37.87147</v>
+      </c>
+      <c r="C312">
+        <v>-122.2617</v>
+      </c>
+      <c r="D312" s="6" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="313">
+      <c r="A313" s="6" t="s">
+        <v>586</v>
+      </c>
+      <c r="B313">
+        <f t="shared" si="2"/>
+        <v>37.87224</v>
+      </c>
+      <c r="C313">
+        <v>-122.25431</v>
+      </c>
+      <c r="D313" s="7" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="314">
+      <c r="A314" s="6" t="s">
+        <v>588</v>
+      </c>
+      <c r="B314">
+        <f t="shared" si="2"/>
+        <v>37.8732</v>
+      </c>
+      <c r="C314">
+        <v>-122.26039</v>
+      </c>
+      <c r="D314" s="7" t="s">
+        <v>589</v>
+      </c>
+    </row>
+    <row r="315">
+      <c r="A315" s="6" t="s">
+        <v>590</v>
+      </c>
+      <c r="B315">
+        <f t="shared" si="2"/>
+        <v>37.87321</v>
+      </c>
+      <c r="C315">
+        <v>-122.26067</v>
+      </c>
+      <c r="D315" s="8" t="s">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="316">
+      <c r="A316" s="6" t="s">
+        <v>592</v>
+      </c>
+      <c r="B316">
+        <f t="shared" si="2"/>
+        <v>37.8676</v>
+      </c>
+      <c r="C316">
+        <v>-122.26521</v>
+      </c>
+      <c r="D316" s="7" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="317">
+      <c r="A317" s="6" t="s">
+        <v>594</v>
+      </c>
+      <c r="B317">
+        <f t="shared" si="2"/>
+        <v>37.87305</v>
+      </c>
+      <c r="C317">
+        <v>-122.26023</v>
+      </c>
+      <c r="D317" s="6" t="s">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="318">
+      <c r="A318" s="6" t="s">
+        <v>596</v>
+      </c>
+      <c r="B318">
+        <f t="shared" si="2"/>
+        <v>37.8696</v>
+      </c>
+      <c r="C318">
+        <v>-122.2615</v>
+      </c>
+      <c r="D318" s="7" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="319">
+      <c r="A319" s="6" t="s">
+        <v>598</v>
+      </c>
+      <c r="B319">
+        <f t="shared" si="2"/>
+        <v>37.86588</v>
+      </c>
+      <c r="C319">
+        <v>-122.25532</v>
+      </c>
+      <c r="D319" s="6" t="s">
+        <v>599</v>
+      </c>
+    </row>
+    <row r="320">
+      <c r="A320" s="6" t="s">
+        <v>600</v>
+      </c>
+      <c r="B320">
+        <f t="shared" si="2"/>
+        <v>37.86936</v>
+      </c>
+      <c r="C320">
+        <v>-122.26013</v>
+      </c>
+      <c r="D320" s="7" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="321">
+      <c r="A321" s="6" t="s">
+        <v>602</v>
+      </c>
+      <c r="B321">
+        <f t="shared" si="2"/>
+        <v>37.87511</v>
+      </c>
+      <c r="C321">
+        <v>-122.25688</v>
+      </c>
+      <c r="D321" s="7" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="322">
+      <c r="A322" s="6" t="s">
+        <v>604</v>
+      </c>
+      <c r="B322">
+        <f t="shared" si="2"/>
+        <v>37.8706</v>
+      </c>
+      <c r="C322">
+        <v>-122.26211</v>
+      </c>
+      <c r="D322" s="7" t="s">
+        <v>605</v>
+      </c>
+    </row>
+    <row r="323">
+      <c r="A323" s="6" t="s">
+        <v>606</v>
+      </c>
+      <c r="B323">
+        <f t="shared" si="2"/>
+        <v>37.87305</v>
+      </c>
+      <c r="C323">
+        <v>-122.26024</v>
+      </c>
+      <c r="D323" s="7" t="s">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="324">
+      <c r="A324" s="6" t="s">
+        <v>608</v>
+      </c>
+      <c r="B324">
+        <f t="shared" si="2"/>
+        <v>37.87443</v>
+      </c>
+      <c r="C324">
+        <v>-122.25821</v>
+      </c>
+      <c r="D324" s="7" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="325">
+      <c r="A325" s="6" t="s">
+        <v>610</v>
+      </c>
+      <c r="B325">
+        <f t="shared" si="2"/>
+        <v>37.87429</v>
+      </c>
+      <c r="C325">
+        <v>-122.25421</v>
+      </c>
+      <c r="D325" s="7" t="s">
+        <v>611</v>
+      </c>
+    </row>
+    <row r="326">
+      <c r="A326" s="6" t="s">
+        <v>612</v>
+      </c>
+      <c r="B326">
+        <f t="shared" si="2"/>
+        <v>37.87238</v>
+      </c>
+      <c r="C326">
+        <v>-122.25968</v>
+      </c>
+      <c r="D326" s="7" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="327">
+      <c r="A327" s="6" t="s">
+        <v>614</v>
+      </c>
+      <c r="B327">
+        <f t="shared" si="2"/>
+        <v>37.87977</v>
+      </c>
+      <c r="C327">
+        <v>-122.25715</v>
+      </c>
+      <c r="D327" s="7" t="s">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="328">
+      <c r="A328" s="6" t="s">
+        <v>616</v>
+      </c>
+      <c r="B328">
+        <f t="shared" si="2"/>
+        <v>37.86293</v>
+      </c>
+      <c r="C328">
+        <v>-122.26414</v>
+      </c>
+      <c r="D328" s="10" t="s">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="329">
+      <c r="A329" s="6" t="s">
+        <v>618</v>
+      </c>
+      <c r="B329">
+        <f t="shared" si="2"/>
+        <v>37.87526</v>
+      </c>
+      <c r="C329">
+        <v>-122.26117</v>
+      </c>
+      <c r="D329" s="6" t="s">
+        <v>619</v>
+      </c>
+    </row>
+    <row r="330">
+      <c r="A330" s="6" t="s">
+        <v>620</v>
+      </c>
+      <c r="B330">
+        <f t="shared" si="2"/>
+        <v>37.86929</v>
+      </c>
+      <c r="C330">
+        <v>-122.26003</v>
+      </c>
+      <c r="D330" s="8" t="s">
+        <v>621</v>
+      </c>
+    </row>
+    <row r="331">
+      <c r="A331" s="6" t="s">
+        <v>622</v>
+      </c>
+      <c r="B331">
+        <f t="shared" si="2"/>
+        <v>37.86564</v>
+      </c>
+      <c r="C331">
+        <v>-122.26893</v>
+      </c>
+      <c r="D331" s="6" t="s">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="332">
+      <c r="A332" s="6" t="s">
+        <v>624</v>
+      </c>
+      <c r="B332">
+        <f t="shared" si="2"/>
+        <v>37.87211</v>
+      </c>
+      <c r="C332">
+        <v>-122.26061</v>
+      </c>
+      <c r="D332" s="7" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="333">
+      <c r="A333" s="6" t="s">
+        <v>625</v>
+      </c>
+      <c r="B333">
+        <f t="shared" si="2"/>
+        <v>37.86405</v>
+      </c>
+      <c r="C333">
+        <v>-122.26401</v>
+      </c>
+      <c r="D333" s="7" t="s">
+        <v>626</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
clustering, more points, no contact info
</commit_message>
<xml_diff>
--- a/src/data/data.xlsx
+++ b/src/data/data.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="637" uniqueCount="627">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="693" uniqueCount="685">
   <si>
     <t>lat</t>
   </si>
@@ -1145,7 +1145,7 @@
     <t>LatLng(37.87016, -122.26217)</t>
   </si>
   <si>
-    <t xml:space="preserve">found out the person i lived didn’t love me back the way i’d hoped </t>
+    <t xml:space="preserve">found out the person i loved didn’t love me back the way i’d hoped </t>
   </si>
   <si>
     <t>LatLng(37.87007, -122.25805)</t>
@@ -1918,6 +1918,180 @@
   </si>
   <si>
     <t>about to bomb an interview in exactly one hour</t>
+  </si>
+  <si>
+    <t>LatLng(37.87279, -122.25477)</t>
+  </si>
+  <si>
+    <t>After finishing a CS midterm that I was afraid I failed, for a class I was retaking</t>
+  </si>
+  <si>
+    <t>LatLng(37.87438, -122.25487)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cried in my dorm room a lot during freshmen year because I was homesick and I felt really alone </t>
+  </si>
+  <si>
+    <t>LatLng(37.86708, -122.25661)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cried when I had learned I got rejected from the same club for the 4th time in a row. </t>
+  </si>
+  <si>
+    <t>LatLng(37.87296, -122.25512)</t>
+  </si>
+  <si>
+    <t>Had a panic attack during midterm. Mind blanked out, felt nauseous, wanted to cry, felt like space was caving in, wanted to bolt out of room. After midterm, ran out of room hyperventilating and wailed outside as all the students trickled out, smiling from how do-able the MT was. Later, professor tells me "you look like you came out of a war zone"</t>
+  </si>
+  <si>
+    <t>LatLng(37.87258, -122.2635)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This past week I got in an argument with my partner. I was waiting for him and he showed up with flowers. I cried out of frustration and joy. </t>
+  </si>
+  <si>
+    <t>LatLng(37.86826, -122.25311)</t>
+  </si>
+  <si>
+    <t>Graduation is approaching and I often get overwhelmed by both the thoughts of what comes next as well as leaving behind people I love.</t>
+  </si>
+  <si>
+    <t>LatLng(37.86875, -122.26012)</t>
+  </si>
+  <si>
+    <t>Had a tough conversation with my mom about my sexuality while I was sitting in the stairwell of Eshleman</t>
+  </si>
+  <si>
+    <t>LatLng(37.86938, -122.25928)</t>
+  </si>
+  <si>
+    <t>Trump won.</t>
+  </si>
+  <si>
+    <t>LatLng(37.86782, -122.25876)</t>
+  </si>
+  <si>
+    <t>The pressure and stress of being a student here really got to me one evening, and it didn't help that my roommate and her friends were being hostile towards me. I facetimed my mom, and I realized I was missing her more than ever. Completely lost it after the call end and cried alone in my room for like 2 hours after that. This took place in Martinez Commons</t>
+  </si>
+  <si>
+    <t>LatLng(37.86306, -122.2578)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">After spending all of spring break back home, my parents dropped me off at my apartment. When they left, I sat all alone in my room where I started crying really hard out of nowhere. Coming back to my apartment reminded me of everything I was dealing with here: feeling so stupid/mediocre/inadequate in Chem 3B and Bio 1A, internal drama with the people I was living with at the time, and just feeling so alone and feeling like I had nobody to go to here. I cried myself to sleep that night. I really wanted to go back home. </t>
+  </si>
+  <si>
+    <t>LatLng(37.87147, -122.26466)</t>
+  </si>
+  <si>
+    <t>I cried today in the ground floor of Tolman Hall.  I cried in between participant sessions for an experiment I'm running.  I cried because of a GSI from hell.  I broke down by myself, and also in the lab of a couple of classmates.  They were supportive, but I also feel like maybe I overwhelmed them.  And then I cried about that, too.</t>
+  </si>
+  <si>
+    <t>LatLng(37.8747, -122.25793)</t>
+  </si>
+  <si>
+    <t>Walking out from Soda Hall after several unproductive hours of trying to work on a project. Midterm scores were released and I was really disappointed with my performance. My hopes of declaring as a CS major were shattered. It was cold and dark out, I felt academically hopeless, and I walked alone. That was the first and only time I've cried on campus. I ended up starting over as CogSci and it's been great -- failure led to something better.</t>
+  </si>
+  <si>
+    <t>LatLng(37.86996, -122.26351)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A Cal Baseball loss. We don’t lose much at home but it hurts to see. </t>
+  </si>
+  <si>
+    <t>LatLng(37.86476, -122.26184)</t>
+  </si>
+  <si>
+    <t>In my room, homesick and missing my family.</t>
+  </si>
+  <si>
+    <t>LatLng(37.86922, -122.26321)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I cried outside of moffit library where everyone was studying because I just couldn’t understand my linguistics homework. I felt like everyone else was getting it and I felt so defeated. </t>
+  </si>
+  <si>
+    <t>LatLng(37.86655, -122.2585)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I was asked by friend if I was okay and I said no, I was honest and felt like I had to open up to someone and let them know how I was feeling. Everyone else around me acted happy, like they had their shit together. I felt alone and was having issues with my roommate, as well as missing my family and thinking how I didn't belong here. </t>
+  </si>
+  <si>
+    <t>LatLng(37.86841, -122.25249)</t>
+  </si>
+  <si>
+    <t>Coming back to college after my mom had passed away. Seeing the dorm where she had moved me in freshman year just broke me.</t>
+  </si>
+  <si>
+    <t>LatLng(37.86967, -122.268)</t>
+  </si>
+  <si>
+    <t>I was PTSD triggered by a song playing at a restaurant that reminded me of one of my child abusers.</t>
+  </si>
+  <si>
+    <t>LatLng(37.86903, -122.25505)</t>
+  </si>
+  <si>
+    <t>Cried in Cafe Strada three times this week. All three times were related to feeling like I didn't understand the material in any of my classes enough to take my midterms and due to the physical issues the insane amount of stress here has given me.</t>
+  </si>
+  <si>
+    <t>LatLng(37.86899, -122.26474)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The other day a girl in my lecture hall rubbed her backpack on me and told me I smelled horrible (4 times in total). People around us noticed, but didn't intervene. She told me I was smelly and worthless. She doesn't seem like she is from around here.  I think she's an international student from China with major princess syndrome (One Child policy?) I used to have tons of international friends in community college. Now, it seems like they really look down on people native to here. I don't understand that. Anyway I struggle with self-esteem issues. This really got to me because it was the first time I ever felt another person regard me as human garbage. </t>
+  </si>
+  <si>
+    <t>LatLng(37.87505, -122.26753)</t>
+  </si>
+  <si>
+    <t>After failing a midterm for a CS class I needed to declare</t>
+  </si>
+  <si>
+    <t>LatLng(37.86896, -122.2562)</t>
+  </si>
+  <si>
+    <t>I had a final on the last day, last time slot of finals week. All my roommates had finished days before that and decided to invite a bunch of people over to our apartment and have a loud party the night before my last final. I tried to tell them to keep it down so I could study, but they obviously didn't care much. I ended up driving to Bancroft, sitting in my car, and studying with only my laptop light. I cried all night while studying.</t>
+  </si>
+  <si>
+    <t>LatLng(37.87213, -122.25882)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Asked a girl to study with me at moffit but she said no.. I even bought her hot cheetos :( </t>
+  </si>
+  <si>
+    <t>LatLng(37.872, -122.25751)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">During my freshman spring, after my very last final had let out from LeConte at 10 PM on Friday. The semester was technically over so people everywhere were celebrating in groups. I messaged everyone I knew but everyone was busy. My entire first year of college had passed by and I still felt so alone. So I cried while walking through campus and Southside. </t>
+  </si>
+  <si>
+    <t>LatLng(37.86821, -122.25936)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Got a text mid lab that my friend, who I really loved, had died of a heroin overdose. I tried to tell my lab partner but I knew if I spoke I would lose it so I just showed her the text. As soon as I said "he was my friend" I started crying in little bursts. I immediately walked out of lab and ended up sobbing in the walgreens with my sunglasses on, and at the bus stop. I had been sober for a long time and had recently started drinking and using again and it was effecting my school performance, my mental health and now my friend was dead. My 5 year relationship was in shambles and its my first semester here at Cal and honestly I hate it. I can't relate to anyone and I feel more alone than I maybe ever have in my life. </t>
+  </si>
+  <si>
+    <t>LatLng(37.86848, -122.26352)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Oh, I was just hella sad and confused. </t>
+  </si>
+  <si>
+    <t>LatLng(37.86976, -122.25269)</t>
+  </si>
+  <si>
+    <t>It was the end of my first semester of law school, and I didn't feel like I had done anything right or that I belonged at school-- and my grades only affirmed that I didn't belong.  I was speaking with a professor about my performance on an exam, and even though I didn't want to be crying, I just started crying.</t>
+  </si>
+  <si>
+    <t>LatLng(37.86591, -122.25487)</t>
+  </si>
+  <si>
+    <t>Unit 2 courtyard at 3 in the morning. I had just failed my second midterm and I came across my ex-boyfriend on social media, whom I missed so much. I felt so defeated.</t>
+  </si>
+  <si>
+    <t>LatLng(37.86962, -122.26061)</t>
+  </si>
+  <si>
+    <t>I was overwhelmed by academics and extracurriculars as a first semester freshman and ended up panic-crying on the balcony behind the Student Learning Center. God bless my roommate who was there for me.</t>
   </si>
 </sst>
 </file>
@@ -4008,7 +4182,7 @@
         <v>232</v>
       </c>
       <c r="B133">
-        <f t="shared" ref="B133:B333" si="2">IFERROR(__xludf.DUMMYFUNCTION("SPLIT(SUBSTITUTE(SUBSTITUTE(A133,""LatLng("",""""), "")"", """"), "","")"),"37.86688")</f>
+        <f t="shared" ref="B133:B361" si="2">IFERROR(__xludf.DUMMYFUNCTION("SPLIT(SUBSTITUTE(SUBSTITUTE(A133,""LatLng("",""""), "")"", """"), "","")"),"37.86688")</f>
         <v>37.86688</v>
       </c>
       <c r="C133">
@@ -5167,7 +5341,7 @@
       <c r="C202">
         <v>-122.26217</v>
       </c>
-      <c r="D202" s="7" t="s">
+      <c r="D202" s="8" t="s">
         <v>370</v>
       </c>
     </row>
@@ -5593,1547 +5767,1967 @@
     </row>
     <row r="231">
       <c r="A231" s="6" t="s">
-        <v>424</v>
+        <v>426</v>
       </c>
       <c r="B231">
         <f t="shared" si="2"/>
-        <v>37.87123</v>
+        <v>37.8718</v>
       </c>
       <c r="C231">
-        <v>-122.25951</v>
+        <v>-122.26013</v>
       </c>
       <c r="D231" s="7" t="s">
-        <v>425</v>
+        <v>427</v>
       </c>
     </row>
     <row r="232">
       <c r="A232" s="6" t="s">
-        <v>426</v>
+        <v>428</v>
       </c>
       <c r="B232">
         <f t="shared" si="2"/>
-        <v>37.8718</v>
+        <v>37.86585</v>
       </c>
       <c r="C232">
-        <v>-122.26013</v>
+        <v>-122.25443</v>
       </c>
       <c r="D232" s="7" t="s">
-        <v>427</v>
+        <v>429</v>
       </c>
     </row>
     <row r="233">
       <c r="A233" s="6" t="s">
-        <v>428</v>
+        <v>430</v>
       </c>
       <c r="B233">
         <f t="shared" si="2"/>
-        <v>37.86585</v>
+        <v>37.87074</v>
       </c>
       <c r="C233">
-        <v>-122.25443</v>
+        <v>-122.25492</v>
       </c>
       <c r="D233" s="7" t="s">
-        <v>429</v>
+        <v>431</v>
       </c>
     </row>
     <row r="234">
       <c r="A234" s="6" t="s">
-        <v>430</v>
+        <v>432</v>
       </c>
       <c r="B234">
         <f t="shared" si="2"/>
-        <v>37.87074</v>
+        <v>37.87297</v>
       </c>
       <c r="C234">
-        <v>-122.25492</v>
+        <v>-122.26011</v>
       </c>
       <c r="D234" s="7" t="s">
-        <v>431</v>
+        <v>433</v>
       </c>
     </row>
     <row r="235">
       <c r="A235" s="6" t="s">
-        <v>432</v>
+        <v>434</v>
       </c>
       <c r="B235">
         <f t="shared" si="2"/>
-        <v>37.87297</v>
+        <v>37.86762</v>
       </c>
       <c r="C235">
-        <v>-122.26011</v>
+        <v>-122.26431</v>
       </c>
       <c r="D235" s="7" t="s">
-        <v>433</v>
+        <v>435</v>
       </c>
     </row>
     <row r="236">
       <c r="A236" s="6" t="s">
-        <v>434</v>
+        <v>436</v>
       </c>
       <c r="B236">
         <f t="shared" si="2"/>
-        <v>37.86762</v>
+        <v>37.8666</v>
       </c>
       <c r="C236">
-        <v>-122.26431</v>
+        <v>-122.25957</v>
       </c>
       <c r="D236" s="7" t="s">
-        <v>435</v>
+        <v>437</v>
       </c>
     </row>
     <row r="237">
       <c r="A237" s="6" t="s">
-        <v>436</v>
+        <v>438</v>
       </c>
       <c r="B237">
         <f t="shared" si="2"/>
-        <v>37.8666</v>
+        <v>37.86953</v>
       </c>
       <c r="C237">
-        <v>-122.25957</v>
-      </c>
-      <c r="D237" s="7" t="s">
-        <v>437</v>
+        <v>-122.26401</v>
+      </c>
+      <c r="D237" s="10" t="s">
+        <v>439</v>
       </c>
     </row>
     <row r="238">
       <c r="A238" s="6" t="s">
-        <v>438</v>
+        <v>440</v>
       </c>
       <c r="B238">
         <f t="shared" si="2"/>
-        <v>37.86953</v>
+        <v>37.8735</v>
       </c>
       <c r="C238">
-        <v>-122.26401</v>
-      </c>
-      <c r="D238" s="10" t="s">
-        <v>439</v>
+        <v>-122.25878</v>
+      </c>
+      <c r="D238" s="7" t="s">
+        <v>441</v>
       </c>
     </row>
     <row r="239">
       <c r="A239" s="6" t="s">
-        <v>440</v>
+        <v>442</v>
       </c>
       <c r="B239">
         <f t="shared" si="2"/>
-        <v>37.8735</v>
+        <v>37.87136</v>
       </c>
       <c r="C239">
-        <v>-122.25878</v>
+        <v>-122.25981</v>
       </c>
       <c r="D239" s="7" t="s">
-        <v>441</v>
+        <v>443</v>
       </c>
     </row>
     <row r="240">
       <c r="A240" s="6" t="s">
-        <v>442</v>
+        <v>444</v>
       </c>
       <c r="B240">
         <f t="shared" si="2"/>
-        <v>37.87136</v>
+        <v>37.87571</v>
       </c>
       <c r="C240">
-        <v>-122.25981</v>
+        <v>-122.25937</v>
       </c>
       <c r="D240" s="7" t="s">
-        <v>443</v>
+        <v>445</v>
       </c>
     </row>
     <row r="241">
       <c r="A241" s="6" t="s">
-        <v>444</v>
+        <v>446</v>
       </c>
       <c r="B241">
         <f t="shared" si="2"/>
-        <v>37.87571</v>
+        <v>37.87135</v>
       </c>
       <c r="C241">
-        <v>-122.25937</v>
+        <v>-122.2681</v>
       </c>
       <c r="D241" s="7" t="s">
-        <v>445</v>
+        <v>447</v>
       </c>
     </row>
     <row r="242">
       <c r="A242" s="6" t="s">
-        <v>446</v>
+        <v>448</v>
       </c>
       <c r="B242">
         <f t="shared" si="2"/>
-        <v>37.87135</v>
+        <v>37.8674</v>
       </c>
       <c r="C242">
-        <v>-122.2681</v>
+        <v>-122.26325</v>
       </c>
       <c r="D242" s="7" t="s">
-        <v>447</v>
+        <v>449</v>
       </c>
     </row>
     <row r="243">
       <c r="A243" s="6" t="s">
-        <v>448</v>
+        <v>450</v>
       </c>
       <c r="B243">
         <f t="shared" si="2"/>
-        <v>37.8674</v>
+        <v>37.86916</v>
       </c>
       <c r="C243">
-        <v>-122.26325</v>
+        <v>-122.25968</v>
       </c>
       <c r="D243" s="7" t="s">
-        <v>449</v>
+        <v>451</v>
       </c>
     </row>
     <row r="244">
       <c r="A244" s="6" t="s">
-        <v>450</v>
+        <v>452</v>
       </c>
       <c r="B244">
         <f t="shared" si="2"/>
-        <v>37.86916</v>
+        <v>37.87008</v>
       </c>
       <c r="C244">
-        <v>-122.25968</v>
+        <v>-122.25525</v>
       </c>
       <c r="D244" s="7" t="s">
-        <v>451</v>
+        <v>453</v>
       </c>
     </row>
     <row r="245">
       <c r="A245" s="6" t="s">
-        <v>452</v>
+        <v>454</v>
       </c>
       <c r="B245">
         <f t="shared" si="2"/>
-        <v>37.87008</v>
+        <v>37.86577</v>
       </c>
       <c r="C245">
-        <v>-122.25525</v>
+        <v>-122.25423</v>
       </c>
       <c r="D245" s="7" t="s">
-        <v>453</v>
+        <v>455</v>
       </c>
     </row>
     <row r="246">
       <c r="A246" s="6" t="s">
-        <v>454</v>
+        <v>456</v>
       </c>
       <c r="B246">
         <f t="shared" si="2"/>
-        <v>37.86577</v>
+        <v>37.87556</v>
       </c>
       <c r="C246">
-        <v>-122.25423</v>
+        <v>-122.25869</v>
       </c>
       <c r="D246" s="7" t="s">
-        <v>455</v>
+        <v>457</v>
       </c>
     </row>
     <row r="247">
       <c r="A247" s="6" t="s">
-        <v>456</v>
+        <v>458</v>
       </c>
       <c r="B247">
         <f t="shared" si="2"/>
-        <v>37.87556</v>
+        <v>37.86713</v>
       </c>
       <c r="C247">
-        <v>-122.25869</v>
+        <v>-122.26083</v>
       </c>
       <c r="D247" s="7" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="248">
       <c r="A248" s="6" t="s">
-        <v>458</v>
+        <v>460</v>
       </c>
       <c r="B248">
         <f t="shared" si="2"/>
-        <v>37.86713</v>
+        <v>37.86726</v>
       </c>
       <c r="C248">
-        <v>-122.26083</v>
+        <v>-122.2644</v>
       </c>
       <c r="D248" s="7" t="s">
-        <v>459</v>
+        <v>461</v>
       </c>
     </row>
     <row r="249">
       <c r="A249" s="6" t="s">
-        <v>460</v>
+        <v>462</v>
       </c>
       <c r="B249">
         <f t="shared" si="2"/>
-        <v>37.86726</v>
+        <v>37.87288</v>
       </c>
       <c r="C249">
-        <v>-122.2644</v>
-      </c>
-      <c r="D249" s="7" t="s">
-        <v>461</v>
+        <v>-122.26225</v>
+      </c>
+      <c r="D249" s="6" t="s">
+        <v>463</v>
       </c>
     </row>
     <row r="250">
       <c r="A250" s="6" t="s">
-        <v>462</v>
+        <v>464</v>
       </c>
       <c r="B250">
         <f t="shared" si="2"/>
-        <v>37.87288</v>
+        <v>37.86939</v>
       </c>
       <c r="C250">
-        <v>-122.26225</v>
+        <v>-122.2598</v>
       </c>
       <c r="D250" s="6" t="s">
-        <v>463</v>
+        <v>465</v>
       </c>
     </row>
     <row r="251">
       <c r="A251" s="6" t="s">
-        <v>464</v>
+        <v>466</v>
       </c>
       <c r="B251">
         <f t="shared" si="2"/>
-        <v>37.86939</v>
+        <v>37.87292</v>
       </c>
       <c r="C251">
-        <v>-122.2598</v>
-      </c>
-      <c r="D251" s="6" t="s">
-        <v>465</v>
+        <v>-122.25561</v>
+      </c>
+      <c r="D251" s="7" t="s">
+        <v>467</v>
       </c>
     </row>
     <row r="252">
       <c r="A252" s="6" t="s">
-        <v>466</v>
+        <v>468</v>
       </c>
       <c r="B252">
         <f t="shared" si="2"/>
-        <v>37.87292</v>
+        <v>37.86562</v>
       </c>
       <c r="C252">
-        <v>-122.25561</v>
+        <v>-122.25361</v>
       </c>
       <c r="D252" s="7" t="s">
-        <v>467</v>
+        <v>469</v>
       </c>
     </row>
     <row r="253">
       <c r="A253" s="6" t="s">
-        <v>468</v>
+        <v>470</v>
       </c>
       <c r="B253">
         <f t="shared" si="2"/>
-        <v>37.86562</v>
+        <v>37.87519</v>
       </c>
       <c r="C253">
-        <v>-122.25361</v>
+        <v>-122.2606</v>
       </c>
       <c r="D253" s="7" t="s">
-        <v>469</v>
+        <v>471</v>
       </c>
     </row>
     <row r="254">
       <c r="A254" s="6" t="s">
-        <v>470</v>
+        <v>472</v>
       </c>
       <c r="B254">
         <f t="shared" si="2"/>
-        <v>37.87519</v>
+        <v>37.87334</v>
       </c>
       <c r="C254">
-        <v>-122.2606</v>
+        <v>-122.25773</v>
       </c>
       <c r="D254" s="7" t="s">
-        <v>471</v>
+        <v>473</v>
       </c>
     </row>
     <row r="255">
       <c r="A255" s="6" t="s">
-        <v>472</v>
+        <v>474</v>
       </c>
       <c r="B255">
         <f t="shared" si="2"/>
-        <v>37.87334</v>
+        <v>37.87383</v>
       </c>
       <c r="C255">
-        <v>-122.25773</v>
+        <v>-122.25663</v>
       </c>
       <c r="D255" s="7" t="s">
-        <v>473</v>
+        <v>475</v>
       </c>
     </row>
     <row r="256">
       <c r="A256" s="6" t="s">
-        <v>474</v>
+        <v>476</v>
       </c>
       <c r="B256">
         <f t="shared" si="2"/>
-        <v>37.87383</v>
+        <v>37.86669</v>
       </c>
       <c r="C256">
-        <v>-122.25663</v>
+        <v>-122.25401</v>
       </c>
       <c r="D256" s="7" t="s">
-        <v>475</v>
+        <v>477</v>
       </c>
     </row>
     <row r="257">
       <c r="A257" s="6" t="s">
-        <v>476</v>
+        <v>478</v>
       </c>
       <c r="B257">
         <f t="shared" si="2"/>
-        <v>37.86669</v>
+        <v>37.86777</v>
       </c>
       <c r="C257">
-        <v>-122.25401</v>
+        <v>-122.26333</v>
       </c>
       <c r="D257" s="7" t="s">
-        <v>477</v>
+        <v>479</v>
       </c>
     </row>
     <row r="258">
       <c r="A258" s="6" t="s">
-        <v>478</v>
+        <v>480</v>
       </c>
       <c r="B258">
         <f t="shared" si="2"/>
-        <v>37.86777</v>
+        <v>37.86909</v>
       </c>
       <c r="C258">
-        <v>-122.26333</v>
-      </c>
-      <c r="D258" s="7" t="s">
-        <v>479</v>
+        <v>-122.26085</v>
+      </c>
+      <c r="D258" s="6" t="s">
+        <v>481</v>
       </c>
     </row>
     <row r="259">
       <c r="A259" s="6" t="s">
-        <v>480</v>
+        <v>482</v>
       </c>
       <c r="B259">
         <f t="shared" si="2"/>
-        <v>37.86909</v>
+        <v>37.86596</v>
       </c>
       <c r="C259">
-        <v>-122.26085</v>
-      </c>
-      <c r="D259" s="6" t="s">
-        <v>481</v>
+        <v>-122.25202</v>
+      </c>
+      <c r="D259" s="7" t="s">
+        <v>483</v>
       </c>
     </row>
     <row r="260">
       <c r="A260" s="6" t="s">
-        <v>482</v>
+        <v>484</v>
       </c>
       <c r="B260">
         <f t="shared" si="2"/>
-        <v>37.86596</v>
+        <v>37.87504</v>
       </c>
       <c r="C260">
-        <v>-122.25202</v>
+        <v>-122.26017</v>
       </c>
       <c r="D260" s="7" t="s">
-        <v>483</v>
+        <v>485</v>
       </c>
     </row>
     <row r="261">
       <c r="A261" s="6" t="s">
-        <v>484</v>
+        <v>486</v>
       </c>
       <c r="B261">
         <f t="shared" si="2"/>
-        <v>37.87504</v>
+        <v>37.87596</v>
       </c>
       <c r="C261">
-        <v>-122.26017</v>
+        <v>-122.2579</v>
       </c>
       <c r="D261" s="7" t="s">
-        <v>485</v>
+        <v>487</v>
       </c>
     </row>
     <row r="262">
       <c r="A262" s="6" t="s">
-        <v>486</v>
+        <v>488</v>
       </c>
       <c r="B262">
         <f t="shared" si="2"/>
-        <v>37.87596</v>
+        <v>37.87547</v>
       </c>
       <c r="C262">
-        <v>-122.2579</v>
-      </c>
-      <c r="D262" s="7" t="s">
-        <v>487</v>
+        <v>-122.25546</v>
+      </c>
+      <c r="D262" s="6" t="s">
+        <v>489</v>
       </c>
     </row>
     <row r="263">
       <c r="A263" s="6" t="s">
-        <v>488</v>
+        <v>490</v>
       </c>
       <c r="B263">
         <f t="shared" si="2"/>
-        <v>37.87547</v>
+        <v>37.86855</v>
       </c>
       <c r="C263">
-        <v>-122.25546</v>
-      </c>
-      <c r="D263" s="6" t="s">
-        <v>489</v>
+        <v>-122.25303</v>
+      </c>
+      <c r="D263" s="8" t="s">
+        <v>491</v>
       </c>
     </row>
     <row r="264">
       <c r="A264" s="6" t="s">
-        <v>490</v>
+        <v>492</v>
       </c>
       <c r="B264">
         <f t="shared" si="2"/>
-        <v>37.86855</v>
+        <v>37.87294</v>
       </c>
       <c r="C264">
-        <v>-122.25303</v>
-      </c>
-      <c r="D264" s="8" t="s">
-        <v>491</v>
+        <v>-122.25313</v>
+      </c>
+      <c r="D264" s="7" t="s">
+        <v>493</v>
       </c>
     </row>
     <row r="265">
       <c r="A265" s="6" t="s">
-        <v>492</v>
+        <v>362</v>
       </c>
       <c r="B265">
         <f t="shared" si="2"/>
-        <v>37.87294</v>
+        <v>37.87147</v>
       </c>
       <c r="C265">
-        <v>-122.25313</v>
+        <v>-122.26434</v>
       </c>
       <c r="D265" s="7" t="s">
-        <v>493</v>
+        <v>494</v>
       </c>
     </row>
     <row r="266">
       <c r="A266" s="6" t="s">
-        <v>362</v>
+        <v>495</v>
       </c>
       <c r="B266">
         <f t="shared" si="2"/>
-        <v>37.87147</v>
+        <v>37.8688</v>
       </c>
       <c r="C266">
-        <v>-122.26434</v>
+        <v>-122.26822</v>
       </c>
       <c r="D266" s="7" t="s">
-        <v>494</v>
+        <v>496</v>
       </c>
     </row>
     <row r="267">
       <c r="A267" s="6" t="s">
-        <v>495</v>
+        <v>497</v>
       </c>
       <c r="B267">
         <f t="shared" si="2"/>
-        <v>37.8688</v>
+        <v>37.87255</v>
       </c>
       <c r="C267">
-        <v>-122.26822</v>
+        <v>-122.25689</v>
       </c>
       <c r="D267" s="7" t="s">
-        <v>496</v>
+        <v>498</v>
       </c>
     </row>
     <row r="268">
       <c r="A268" s="6" t="s">
-        <v>497</v>
+        <v>499</v>
       </c>
       <c r="B268">
         <f t="shared" si="2"/>
-        <v>37.87255</v>
+        <v>37.87018</v>
       </c>
       <c r="C268">
-        <v>-122.25689</v>
+        <v>-122.25972</v>
       </c>
       <c r="D268" s="7" t="s">
-        <v>498</v>
+        <v>500</v>
       </c>
     </row>
     <row r="269">
       <c r="A269" s="6" t="s">
-        <v>499</v>
+        <v>501</v>
       </c>
       <c r="B269">
         <f t="shared" si="2"/>
-        <v>37.87018</v>
+        <v>37.87243</v>
       </c>
       <c r="C269">
-        <v>-122.25972</v>
+        <v>-122.25843</v>
       </c>
       <c r="D269" s="7" t="s">
-        <v>500</v>
+        <v>502</v>
       </c>
     </row>
     <row r="270">
       <c r="A270" s="6" t="s">
-        <v>501</v>
+        <v>503</v>
       </c>
       <c r="B270">
         <f t="shared" si="2"/>
-        <v>37.87243</v>
+        <v>37.86611</v>
       </c>
       <c r="C270">
-        <v>-122.25843</v>
+        <v>-122.2559</v>
       </c>
       <c r="D270" s="7" t="s">
-        <v>502</v>
+        <v>504</v>
       </c>
     </row>
     <row r="271">
       <c r="A271" s="6" t="s">
-        <v>503</v>
+        <v>505</v>
       </c>
       <c r="B271">
         <f t="shared" si="2"/>
-        <v>37.86611</v>
+        <v>37.86784</v>
       </c>
       <c r="C271">
-        <v>-122.2559</v>
+        <v>-122.25122</v>
       </c>
       <c r="D271" s="7" t="s">
-        <v>504</v>
+        <v>506</v>
       </c>
     </row>
     <row r="272">
       <c r="A272" s="6" t="s">
-        <v>505</v>
+        <v>507</v>
       </c>
       <c r="B272">
         <f t="shared" si="2"/>
-        <v>37.86784</v>
+        <v>37.87197</v>
       </c>
       <c r="C272">
-        <v>-122.25122</v>
+        <v>-122.25779</v>
       </c>
       <c r="D272" s="7" t="s">
-        <v>506</v>
+        <v>508</v>
       </c>
     </row>
     <row r="273">
       <c r="A273" s="6" t="s">
-        <v>507</v>
+        <v>242</v>
       </c>
       <c r="B273">
         <f t="shared" si="2"/>
-        <v>37.87197</v>
+        <v>37.87148</v>
       </c>
       <c r="C273">
-        <v>-122.25779</v>
-      </c>
-      <c r="D273" s="7" t="s">
-        <v>508</v>
+        <v>-122.26466</v>
+      </c>
+      <c r="D273" s="6" t="s">
+        <v>509</v>
       </c>
     </row>
     <row r="274">
       <c r="A274" s="6" t="s">
-        <v>242</v>
+        <v>510</v>
       </c>
       <c r="B274">
         <f t="shared" si="2"/>
-        <v>37.87148</v>
+        <v>37.86611</v>
       </c>
       <c r="C274">
-        <v>-122.26466</v>
-      </c>
-      <c r="D274" s="6" t="s">
-        <v>509</v>
+        <v>-122.25483</v>
+      </c>
+      <c r="D274" s="7" t="s">
+        <v>511</v>
       </c>
     </row>
     <row r="275">
       <c r="A275" s="6" t="s">
-        <v>510</v>
+        <v>512</v>
       </c>
       <c r="B275">
         <f t="shared" si="2"/>
-        <v>37.86611</v>
+        <v>37.8681</v>
       </c>
       <c r="C275">
-        <v>-122.25483</v>
-      </c>
-      <c r="D275" s="7" t="s">
-        <v>511</v>
+        <v>-122.255</v>
+      </c>
+      <c r="D275" s="6" t="s">
+        <v>513</v>
       </c>
     </row>
     <row r="276">
       <c r="A276" s="6" t="s">
-        <v>512</v>
+        <v>514</v>
       </c>
       <c r="B276">
         <f t="shared" si="2"/>
-        <v>37.8681</v>
+        <v>37.87223</v>
       </c>
       <c r="C276">
-        <v>-122.255</v>
-      </c>
-      <c r="D276" s="6" t="s">
-        <v>513</v>
+        <v>-122.25584</v>
+      </c>
+      <c r="D276" s="7" t="s">
+        <v>515</v>
       </c>
     </row>
     <row r="277">
       <c r="A277" s="6" t="s">
-        <v>514</v>
+        <v>516</v>
       </c>
       <c r="B277">
         <f t="shared" si="2"/>
-        <v>37.87223</v>
+        <v>37.87323</v>
       </c>
       <c r="C277">
-        <v>-122.25584</v>
+        <v>-122.25301</v>
       </c>
       <c r="D277" s="7" t="s">
-        <v>515</v>
+        <v>517</v>
       </c>
     </row>
     <row r="278">
       <c r="A278" s="6" t="s">
-        <v>516</v>
+        <v>518</v>
       </c>
       <c r="B278">
         <f t="shared" si="2"/>
-        <v>37.87323</v>
+        <v>37.868</v>
       </c>
       <c r="C278">
-        <v>-122.25301</v>
+        <v>-122.25545</v>
       </c>
       <c r="D278" s="7" t="s">
-        <v>517</v>
+        <v>519</v>
       </c>
     </row>
     <row r="279">
       <c r="A279" s="6" t="s">
-        <v>518</v>
+        <v>520</v>
       </c>
       <c r="B279">
         <f t="shared" si="2"/>
-        <v>37.868</v>
+        <v>37.87288</v>
       </c>
       <c r="C279">
-        <v>-122.25545</v>
+        <v>-122.25715</v>
       </c>
       <c r="D279" s="7" t="s">
-        <v>519</v>
+        <v>521</v>
       </c>
     </row>
     <row r="280">
       <c r="A280" s="6" t="s">
-        <v>520</v>
+        <v>522</v>
       </c>
       <c r="B280">
         <f t="shared" si="2"/>
-        <v>37.87288</v>
+        <v>37.86906</v>
       </c>
       <c r="C280">
-        <v>-122.25715</v>
+        <v>-122.262</v>
       </c>
       <c r="D280" s="7" t="s">
-        <v>521</v>
+        <v>523</v>
       </c>
     </row>
     <row r="281">
       <c r="A281" s="6" t="s">
-        <v>522</v>
+        <v>524</v>
       </c>
       <c r="B281">
         <f t="shared" si="2"/>
-        <v>37.86906</v>
+        <v>37.86981</v>
       </c>
       <c r="C281">
-        <v>-122.262</v>
+        <v>-122.25512</v>
       </c>
       <c r="D281" s="7" t="s">
-        <v>523</v>
+        <v>525</v>
       </c>
     </row>
     <row r="282">
       <c r="A282" s="6" t="s">
-        <v>524</v>
+        <v>526</v>
       </c>
       <c r="B282">
         <f t="shared" si="2"/>
-        <v>37.86981</v>
+        <v>37.86573</v>
       </c>
       <c r="C282">
-        <v>-122.25512</v>
+        <v>-122.24643</v>
       </c>
       <c r="D282" s="7" t="s">
-        <v>525</v>
+        <v>527</v>
       </c>
     </row>
     <row r="283">
       <c r="A283" s="6" t="s">
-        <v>526</v>
+        <v>528</v>
       </c>
       <c r="B283">
         <f t="shared" si="2"/>
-        <v>37.86573</v>
+        <v>37.86882</v>
       </c>
       <c r="C283">
-        <v>-122.24643</v>
+        <v>-122.25246</v>
       </c>
       <c r="D283" s="7" t="s">
-        <v>527</v>
+        <v>529</v>
       </c>
     </row>
     <row r="284">
       <c r="A284" s="6" t="s">
-        <v>528</v>
+        <v>530</v>
       </c>
       <c r="B284">
         <f t="shared" si="2"/>
-        <v>37.86882</v>
+        <v>37.86493</v>
       </c>
       <c r="C284">
-        <v>-122.25246</v>
+        <v>-122.24895</v>
       </c>
       <c r="D284" s="7" t="s">
-        <v>529</v>
+        <v>531</v>
       </c>
     </row>
     <row r="285">
       <c r="A285" s="6" t="s">
-        <v>530</v>
+        <v>532</v>
       </c>
       <c r="B285">
         <f t="shared" si="2"/>
-        <v>37.86493</v>
+        <v>37.86455</v>
       </c>
       <c r="C285">
-        <v>-122.24895</v>
+        <v>-122.26225</v>
       </c>
       <c r="D285" s="7" t="s">
-        <v>531</v>
+        <v>533</v>
       </c>
     </row>
     <row r="286">
       <c r="A286" s="6" t="s">
-        <v>532</v>
+        <v>534</v>
       </c>
       <c r="B286">
         <f t="shared" si="2"/>
-        <v>37.86455</v>
+        <v>37.87057</v>
       </c>
       <c r="C286">
-        <v>-122.26225</v>
+        <v>-122.25395</v>
       </c>
       <c r="D286" s="7" t="s">
-        <v>533</v>
+        <v>535</v>
       </c>
     </row>
     <row r="287">
       <c r="A287" s="6" t="s">
-        <v>534</v>
+        <v>536</v>
       </c>
       <c r="B287">
         <f t="shared" si="2"/>
-        <v>37.87057</v>
+        <v>37.87425</v>
       </c>
       <c r="C287">
-        <v>-122.25395</v>
-      </c>
-      <c r="D287" s="7" t="s">
-        <v>535</v>
+        <v>-122.25732</v>
+      </c>
+      <c r="D287" s="6" t="s">
+        <v>537</v>
       </c>
     </row>
     <row r="288">
       <c r="A288" s="6" t="s">
-        <v>536</v>
+        <v>538</v>
       </c>
       <c r="B288">
         <f t="shared" si="2"/>
-        <v>37.87425</v>
+        <v>37.86881</v>
       </c>
       <c r="C288">
-        <v>-122.25732</v>
-      </c>
-      <c r="D288" s="6" t="s">
-        <v>537</v>
+        <v>-122.25777</v>
+      </c>
+      <c r="D288" s="7" t="s">
+        <v>539</v>
       </c>
     </row>
     <row r="289">
       <c r="A289" s="6" t="s">
-        <v>538</v>
+        <v>540</v>
       </c>
       <c r="B289">
         <f t="shared" si="2"/>
-        <v>37.86881</v>
+        <v>37.87336</v>
       </c>
       <c r="C289">
-        <v>-122.25777</v>
+        <v>-122.25483</v>
       </c>
       <c r="D289" s="7" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
     </row>
     <row r="290">
       <c r="A290" s="6" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
       <c r="B290">
         <f t="shared" si="2"/>
-        <v>37.87336</v>
+        <v>37.87089</v>
       </c>
       <c r="C290">
-        <v>-122.25483</v>
+        <v>-122.25286</v>
       </c>
       <c r="D290" s="7" t="s">
-        <v>541</v>
+        <v>543</v>
       </c>
     </row>
     <row r="291">
       <c r="A291" s="6" t="s">
-        <v>542</v>
+        <v>544</v>
       </c>
       <c r="B291">
         <f t="shared" si="2"/>
-        <v>37.87089</v>
+        <v>37.87001</v>
       </c>
       <c r="C291">
-        <v>-122.25286</v>
+        <v>-122.25797</v>
       </c>
       <c r="D291" s="7" t="s">
-        <v>543</v>
+        <v>545</v>
       </c>
     </row>
     <row r="292">
       <c r="A292" s="6" t="s">
-        <v>544</v>
+        <v>546</v>
       </c>
       <c r="B292">
         <f t="shared" si="2"/>
-        <v>37.87001</v>
+        <v>37.86777</v>
       </c>
       <c r="C292">
-        <v>-122.25797</v>
+        <v>-122.25161</v>
       </c>
       <c r="D292" s="7" t="s">
-        <v>545</v>
+        <v>547</v>
       </c>
     </row>
     <row r="293">
       <c r="A293" s="6" t="s">
-        <v>546</v>
+        <v>548</v>
       </c>
       <c r="B293">
         <f t="shared" si="2"/>
-        <v>37.86777</v>
+        <v>37.86771</v>
       </c>
       <c r="C293">
-        <v>-122.25161</v>
+        <v>-122.252</v>
       </c>
       <c r="D293" s="7" t="s">
-        <v>547</v>
+        <v>549</v>
       </c>
     </row>
     <row r="294">
       <c r="A294" s="6" t="s">
-        <v>548</v>
+        <v>550</v>
       </c>
       <c r="B294">
         <f t="shared" si="2"/>
-        <v>37.86771</v>
+        <v>37.87172</v>
       </c>
       <c r="C294">
-        <v>-122.252</v>
+        <v>-122.25818</v>
       </c>
       <c r="D294" s="7" t="s">
-        <v>549</v>
+        <v>551</v>
       </c>
     </row>
     <row r="295">
       <c r="A295" s="6" t="s">
-        <v>550</v>
+        <v>552</v>
       </c>
       <c r="B295">
         <f t="shared" si="2"/>
-        <v>37.87172</v>
+        <v>37.86778</v>
       </c>
       <c r="C295">
-        <v>-122.25818</v>
+        <v>-122.25187</v>
       </c>
       <c r="D295" s="7" t="s">
-        <v>551</v>
+        <v>553</v>
       </c>
     </row>
     <row r="296">
       <c r="A296" s="6" t="s">
-        <v>552</v>
+        <v>554</v>
       </c>
       <c r="B296">
         <f t="shared" si="2"/>
-        <v>37.86778</v>
+        <v>37.87258</v>
       </c>
       <c r="C296">
-        <v>-122.25187</v>
-      </c>
-      <c r="D296" s="7" t="s">
-        <v>553</v>
+        <v>-122.26753</v>
+      </c>
+      <c r="D296" s="10" t="s">
+        <v>555</v>
       </c>
     </row>
     <row r="297">
       <c r="A297" s="6" t="s">
-        <v>554</v>
+        <v>556</v>
       </c>
       <c r="B297">
         <f t="shared" si="2"/>
-        <v>37.87258</v>
+        <v>37.8653</v>
       </c>
       <c r="C297">
-        <v>-122.26753</v>
-      </c>
-      <c r="D297" s="10" t="s">
-        <v>555</v>
+        <v>-122.24972</v>
+      </c>
+      <c r="D297" s="8" t="s">
+        <v>557</v>
       </c>
     </row>
     <row r="298">
       <c r="A298" s="6" t="s">
-        <v>556</v>
+        <v>558</v>
       </c>
       <c r="B298">
         <f t="shared" si="2"/>
-        <v>37.8653</v>
+        <v>37.86933</v>
       </c>
       <c r="C298">
-        <v>-122.24972</v>
-      </c>
-      <c r="D298" s="8" t="s">
-        <v>557</v>
+        <v>-122.255</v>
+      </c>
+      <c r="D298" s="6" t="s">
+        <v>559</v>
       </c>
     </row>
     <row r="299">
       <c r="A299" s="6" t="s">
-        <v>558</v>
+        <v>560</v>
       </c>
       <c r="B299">
         <f t="shared" si="2"/>
-        <v>37.86933</v>
+        <v>37.87346</v>
       </c>
       <c r="C299">
-        <v>-122.255</v>
-      </c>
-      <c r="D299" s="6" t="s">
-        <v>559</v>
+        <v>-122.25793</v>
+      </c>
+      <c r="D299" s="7" t="s">
+        <v>561</v>
       </c>
     </row>
     <row r="300">
       <c r="A300" s="6" t="s">
-        <v>560</v>
+        <v>562</v>
       </c>
       <c r="B300">
         <f t="shared" si="2"/>
-        <v>37.87346</v>
+        <v>37.86838</v>
       </c>
       <c r="C300">
-        <v>-122.25793</v>
+        <v>-122.26057</v>
       </c>
       <c r="D300" s="7" t="s">
-        <v>561</v>
+        <v>563</v>
       </c>
     </row>
     <row r="301">
       <c r="A301" s="6" t="s">
-        <v>562</v>
+        <v>564</v>
       </c>
       <c r="B301">
         <f t="shared" si="2"/>
-        <v>37.86838</v>
+        <v>37.86239</v>
       </c>
       <c r="C301">
-        <v>-122.26057</v>
+        <v>-122.26101</v>
       </c>
       <c r="D301" s="7" t="s">
-        <v>563</v>
+        <v>565</v>
       </c>
     </row>
     <row r="302">
       <c r="A302" s="6" t="s">
-        <v>564</v>
+        <v>566</v>
       </c>
       <c r="B302">
         <f t="shared" si="2"/>
-        <v>37.86239</v>
+        <v>37.86998</v>
       </c>
       <c r="C302">
-        <v>-122.26101</v>
-      </c>
-      <c r="D302" s="7" t="s">
-        <v>565</v>
+        <v>-122.25802</v>
+      </c>
+      <c r="D302" s="6" t="s">
+        <v>567</v>
       </c>
     </row>
     <row r="303">
       <c r="A303" s="6" t="s">
-        <v>566</v>
+        <v>568</v>
       </c>
       <c r="B303">
         <f t="shared" si="2"/>
-        <v>37.86998</v>
+        <v>37.87228</v>
       </c>
       <c r="C303">
-        <v>-122.25802</v>
-      </c>
-      <c r="D303" s="6" t="s">
-        <v>567</v>
+        <v>-122.25996</v>
+      </c>
+      <c r="D303" s="7" t="s">
+        <v>569</v>
       </c>
     </row>
     <row r="304">
       <c r="A304" s="6" t="s">
-        <v>568</v>
+        <v>570</v>
       </c>
       <c r="B304">
         <f t="shared" si="2"/>
-        <v>37.87228</v>
+        <v>37.87153</v>
       </c>
       <c r="C304">
-        <v>-122.25996</v>
+        <v>-122.26277</v>
       </c>
       <c r="D304" s="7" t="s">
-        <v>569</v>
+        <v>571</v>
       </c>
     </row>
     <row r="305">
       <c r="A305" s="6" t="s">
-        <v>570</v>
+        <v>572</v>
       </c>
       <c r="B305">
         <f t="shared" si="2"/>
-        <v>37.87153</v>
+        <v>37.87377</v>
       </c>
       <c r="C305">
-        <v>-122.26277</v>
+        <v>-122.26367</v>
       </c>
       <c r="D305" s="7" t="s">
-        <v>571</v>
+        <v>573</v>
       </c>
     </row>
     <row r="306">
       <c r="A306" s="6" t="s">
-        <v>572</v>
+        <v>574</v>
       </c>
       <c r="B306">
         <f t="shared" si="2"/>
-        <v>37.87377</v>
+        <v>37.87133</v>
       </c>
       <c r="C306">
-        <v>-122.26367</v>
-      </c>
-      <c r="D306" s="7" t="s">
-        <v>573</v>
+        <v>-122.25011</v>
+      </c>
+      <c r="D306" s="10" t="s">
+        <v>575</v>
       </c>
     </row>
     <row r="307">
       <c r="A307" s="6" t="s">
-        <v>574</v>
+        <v>576</v>
       </c>
       <c r="B307">
         <f t="shared" si="2"/>
-        <v>37.87133</v>
+        <v>37.86985</v>
       </c>
       <c r="C307">
-        <v>-122.25011</v>
-      </c>
-      <c r="D307" s="10" t="s">
-        <v>575</v>
+        <v>-122.25928</v>
+      </c>
+      <c r="D307" s="7" t="s">
+        <v>577</v>
       </c>
     </row>
     <row r="308">
       <c r="A308" s="6" t="s">
-        <v>576</v>
+        <v>578</v>
       </c>
       <c r="B308">
         <f t="shared" si="2"/>
-        <v>37.86985</v>
+        <v>37.86952</v>
       </c>
       <c r="C308">
-        <v>-122.25928</v>
+        <v>-122.267</v>
       </c>
       <c r="D308" s="7" t="s">
-        <v>577</v>
+        <v>579</v>
       </c>
     </row>
     <row r="309">
       <c r="A309" s="6" t="s">
-        <v>578</v>
+        <v>580</v>
       </c>
       <c r="B309">
         <f t="shared" si="2"/>
-        <v>37.86952</v>
+        <v>37.86961</v>
       </c>
       <c r="C309">
-        <v>-122.267</v>
+        <v>-122.26661</v>
       </c>
       <c r="D309" s="7" t="s">
-        <v>579</v>
+        <v>581</v>
       </c>
     </row>
     <row r="310">
       <c r="A310" s="6" t="s">
-        <v>580</v>
+        <v>582</v>
       </c>
       <c r="B310">
         <f t="shared" si="2"/>
-        <v>37.86961</v>
+        <v>37.86812</v>
       </c>
       <c r="C310">
-        <v>-122.26661</v>
+        <v>-122.25504</v>
       </c>
       <c r="D310" s="7" t="s">
-        <v>581</v>
+        <v>583</v>
       </c>
     </row>
     <row r="311">
       <c r="A311" s="6" t="s">
-        <v>582</v>
+        <v>584</v>
       </c>
       <c r="B311">
         <f t="shared" si="2"/>
-        <v>37.86812</v>
+        <v>37.87147</v>
       </c>
       <c r="C311">
-        <v>-122.25504</v>
-      </c>
-      <c r="D311" s="7" t="s">
-        <v>583</v>
+        <v>-122.2617</v>
+      </c>
+      <c r="D311" s="6" t="s">
+        <v>585</v>
       </c>
     </row>
     <row r="312">
       <c r="A312" s="6" t="s">
-        <v>584</v>
+        <v>586</v>
       </c>
       <c r="B312">
         <f t="shared" si="2"/>
-        <v>37.87147</v>
+        <v>37.87224</v>
       </c>
       <c r="C312">
-        <v>-122.2617</v>
-      </c>
-      <c r="D312" s="6" t="s">
-        <v>585</v>
+        <v>-122.25431</v>
+      </c>
+      <c r="D312" s="7" t="s">
+        <v>587</v>
       </c>
     </row>
     <row r="313">
       <c r="A313" s="6" t="s">
-        <v>586</v>
+        <v>588</v>
       </c>
       <c r="B313">
         <f t="shared" si="2"/>
-        <v>37.87224</v>
+        <v>37.8732</v>
       </c>
       <c r="C313">
-        <v>-122.25431</v>
+        <v>-122.26039</v>
       </c>
       <c r="D313" s="7" t="s">
-        <v>587</v>
+        <v>589</v>
       </c>
     </row>
     <row r="314">
       <c r="A314" s="6" t="s">
-        <v>588</v>
+        <v>590</v>
       </c>
       <c r="B314">
         <f t="shared" si="2"/>
-        <v>37.8732</v>
+        <v>37.87321</v>
       </c>
       <c r="C314">
-        <v>-122.26039</v>
-      </c>
-      <c r="D314" s="7" t="s">
-        <v>589</v>
+        <v>-122.26067</v>
+      </c>
+      <c r="D314" s="8" t="s">
+        <v>591</v>
       </c>
     </row>
     <row r="315">
       <c r="A315" s="6" t="s">
-        <v>590</v>
+        <v>592</v>
       </c>
       <c r="B315">
         <f t="shared" si="2"/>
-        <v>37.87321</v>
+        <v>37.8676</v>
       </c>
       <c r="C315">
-        <v>-122.26067</v>
-      </c>
-      <c r="D315" s="8" t="s">
-        <v>591</v>
+        <v>-122.26521</v>
+      </c>
+      <c r="D315" s="7" t="s">
+        <v>593</v>
       </c>
     </row>
     <row r="316">
       <c r="A316" s="6" t="s">
-        <v>592</v>
+        <v>594</v>
       </c>
       <c r="B316">
         <f t="shared" si="2"/>
-        <v>37.8676</v>
+        <v>37.87305</v>
       </c>
       <c r="C316">
-        <v>-122.26521</v>
-      </c>
-      <c r="D316" s="7" t="s">
-        <v>593</v>
+        <v>-122.26023</v>
+      </c>
+      <c r="D316" s="6" t="s">
+        <v>595</v>
       </c>
     </row>
     <row r="317">
       <c r="A317" s="6" t="s">
-        <v>594</v>
+        <v>596</v>
       </c>
       <c r="B317">
         <f t="shared" si="2"/>
-        <v>37.87305</v>
+        <v>37.8696</v>
       </c>
       <c r="C317">
-        <v>-122.26023</v>
-      </c>
-      <c r="D317" s="6" t="s">
-        <v>595</v>
+        <v>-122.2615</v>
+      </c>
+      <c r="D317" s="7" t="s">
+        <v>597</v>
       </c>
     </row>
     <row r="318">
       <c r="A318" s="6" t="s">
-        <v>596</v>
+        <v>598</v>
       </c>
       <c r="B318">
         <f t="shared" si="2"/>
-        <v>37.8696</v>
+        <v>37.86588</v>
       </c>
       <c r="C318">
-        <v>-122.2615</v>
-      </c>
-      <c r="D318" s="7" t="s">
-        <v>597</v>
+        <v>-122.25532</v>
+      </c>
+      <c r="D318" s="6" t="s">
+        <v>599</v>
       </c>
     </row>
     <row r="319">
       <c r="A319" s="6" t="s">
-        <v>598</v>
+        <v>600</v>
       </c>
       <c r="B319">
         <f t="shared" si="2"/>
-        <v>37.86588</v>
+        <v>37.86936</v>
       </c>
       <c r="C319">
-        <v>-122.25532</v>
-      </c>
-      <c r="D319" s="6" t="s">
-        <v>599</v>
+        <v>-122.26013</v>
+      </c>
+      <c r="D319" s="7" t="s">
+        <v>601</v>
       </c>
     </row>
     <row r="320">
       <c r="A320" s="6" t="s">
-        <v>600</v>
+        <v>602</v>
       </c>
       <c r="B320">
         <f t="shared" si="2"/>
-        <v>37.86936</v>
+        <v>37.87511</v>
       </c>
       <c r="C320">
-        <v>-122.26013</v>
+        <v>-122.25688</v>
       </c>
       <c r="D320" s="7" t="s">
-        <v>601</v>
+        <v>603</v>
       </c>
     </row>
     <row r="321">
       <c r="A321" s="6" t="s">
-        <v>602</v>
+        <v>604</v>
       </c>
       <c r="B321">
         <f t="shared" si="2"/>
-        <v>37.87511</v>
+        <v>37.8706</v>
       </c>
       <c r="C321">
-        <v>-122.25688</v>
+        <v>-122.26211</v>
       </c>
       <c r="D321" s="7" t="s">
-        <v>603</v>
+        <v>605</v>
       </c>
     </row>
     <row r="322">
       <c r="A322" s="6" t="s">
-        <v>604</v>
+        <v>606</v>
       </c>
       <c r="B322">
         <f t="shared" si="2"/>
-        <v>37.8706</v>
+        <v>37.87305</v>
       </c>
       <c r="C322">
-        <v>-122.26211</v>
+        <v>-122.26024</v>
       </c>
       <c r="D322" s="7" t="s">
-        <v>605</v>
+        <v>607</v>
       </c>
     </row>
     <row r="323">
       <c r="A323" s="6" t="s">
-        <v>606</v>
+        <v>608</v>
       </c>
       <c r="B323">
         <f t="shared" si="2"/>
-        <v>37.87305</v>
+        <v>37.87443</v>
       </c>
       <c r="C323">
-        <v>-122.26024</v>
+        <v>-122.25821</v>
       </c>
       <c r="D323" s="7" t="s">
-        <v>607</v>
+        <v>609</v>
       </c>
     </row>
     <row r="324">
       <c r="A324" s="6" t="s">
-        <v>608</v>
+        <v>610</v>
       </c>
       <c r="B324">
         <f t="shared" si="2"/>
-        <v>37.87443</v>
+        <v>37.87429</v>
       </c>
       <c r="C324">
-        <v>-122.25821</v>
+        <v>-122.25421</v>
       </c>
       <c r="D324" s="7" t="s">
-        <v>609</v>
+        <v>611</v>
       </c>
     </row>
     <row r="325">
       <c r="A325" s="6" t="s">
-        <v>610</v>
+        <v>612</v>
       </c>
       <c r="B325">
         <f t="shared" si="2"/>
-        <v>37.87429</v>
+        <v>37.87238</v>
       </c>
       <c r="C325">
-        <v>-122.25421</v>
+        <v>-122.25968</v>
       </c>
       <c r="D325" s="7" t="s">
-        <v>611</v>
+        <v>613</v>
       </c>
     </row>
     <row r="326">
       <c r="A326" s="6" t="s">
-        <v>612</v>
+        <v>614</v>
       </c>
       <c r="B326">
         <f t="shared" si="2"/>
-        <v>37.87238</v>
+        <v>37.87977</v>
       </c>
       <c r="C326">
-        <v>-122.25968</v>
+        <v>-122.25715</v>
       </c>
       <c r="D326" s="7" t="s">
-        <v>613</v>
+        <v>615</v>
       </c>
     </row>
     <row r="327">
       <c r="A327" s="6" t="s">
-        <v>614</v>
+        <v>616</v>
       </c>
       <c r="B327">
         <f t="shared" si="2"/>
-        <v>37.87977</v>
+        <v>37.86293</v>
       </c>
       <c r="C327">
-        <v>-122.25715</v>
-      </c>
-      <c r="D327" s="7" t="s">
-        <v>615</v>
+        <v>-122.26414</v>
+      </c>
+      <c r="D327" s="10" t="s">
+        <v>617</v>
       </c>
     </row>
     <row r="328">
       <c r="A328" s="6" t="s">
-        <v>616</v>
+        <v>618</v>
       </c>
       <c r="B328">
         <f t="shared" si="2"/>
-        <v>37.86293</v>
+        <v>37.87526</v>
       </c>
       <c r="C328">
-        <v>-122.26414</v>
-      </c>
-      <c r="D328" s="10" t="s">
-        <v>617</v>
+        <v>-122.26117</v>
+      </c>
+      <c r="D328" s="6" t="s">
+        <v>619</v>
       </c>
     </row>
     <row r="329">
       <c r="A329" s="6" t="s">
-        <v>618</v>
+        <v>620</v>
       </c>
       <c r="B329">
         <f t="shared" si="2"/>
-        <v>37.87526</v>
+        <v>37.86929</v>
       </c>
       <c r="C329">
-        <v>-122.26117</v>
-      </c>
-      <c r="D329" s="6" t="s">
-        <v>619</v>
+        <v>-122.26003</v>
+      </c>
+      <c r="D329" s="8" t="s">
+        <v>621</v>
       </c>
     </row>
     <row r="330">
       <c r="A330" s="6" t="s">
-        <v>620</v>
+        <v>622</v>
       </c>
       <c r="B330">
         <f t="shared" si="2"/>
-        <v>37.86929</v>
+        <v>37.86564</v>
       </c>
       <c r="C330">
-        <v>-122.26003</v>
-      </c>
-      <c r="D330" s="8" t="s">
-        <v>621</v>
+        <v>-122.26893</v>
+      </c>
+      <c r="D330" s="6" t="s">
+        <v>623</v>
       </c>
     </row>
     <row r="331">
       <c r="A331" s="6" t="s">
-        <v>622</v>
+        <v>624</v>
       </c>
       <c r="B331">
         <f t="shared" si="2"/>
-        <v>37.86564</v>
+        <v>37.87211</v>
       </c>
       <c r="C331">
-        <v>-122.26893</v>
-      </c>
-      <c r="D331" s="6" t="s">
-        <v>623</v>
+        <v>-122.26061</v>
+      </c>
+      <c r="D331" s="7" t="s">
+        <v>441</v>
       </c>
     </row>
     <row r="332">
       <c r="A332" s="6" t="s">
-        <v>624</v>
+        <v>625</v>
       </c>
       <c r="B332">
         <f t="shared" si="2"/>
-        <v>37.87211</v>
+        <v>37.86405</v>
       </c>
       <c r="C332">
-        <v>-122.26061</v>
+        <v>-122.26401</v>
       </c>
       <c r="D332" s="7" t="s">
-        <v>441</v>
+        <v>626</v>
       </c>
     </row>
     <row r="333">
       <c r="A333" s="6" t="s">
-        <v>625</v>
+        <v>627</v>
       </c>
       <c r="B333">
         <f t="shared" si="2"/>
-        <v>37.86405</v>
+        <v>37.87279</v>
       </c>
       <c r="C333">
-        <v>-122.26401</v>
+        <v>-122.25477</v>
       </c>
       <c r="D333" s="7" t="s">
-        <v>626</v>
+        <v>628</v>
+      </c>
+    </row>
+    <row r="334">
+      <c r="A334" s="6" t="s">
+        <v>629</v>
+      </c>
+      <c r="B334">
+        <f t="shared" si="2"/>
+        <v>37.87438</v>
+      </c>
+      <c r="C334">
+        <v>-122.25487</v>
+      </c>
+      <c r="D334" s="7" t="s">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="335">
+      <c r="A335" s="6" t="s">
+        <v>631</v>
+      </c>
+      <c r="B335">
+        <f t="shared" si="2"/>
+        <v>37.86708</v>
+      </c>
+      <c r="C335">
+        <v>-122.25661</v>
+      </c>
+      <c r="D335" s="7" t="s">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="336">
+      <c r="A336" s="6" t="s">
+        <v>633</v>
+      </c>
+      <c r="B336">
+        <f t="shared" si="2"/>
+        <v>37.87296</v>
+      </c>
+      <c r="C336">
+        <v>-122.25512</v>
+      </c>
+      <c r="D336" s="7" t="s">
+        <v>634</v>
+      </c>
+    </row>
+    <row r="337">
+      <c r="A337" s="6" t="s">
+        <v>635</v>
+      </c>
+      <c r="B337">
+        <f t="shared" si="2"/>
+        <v>37.87258</v>
+      </c>
+      <c r="C337">
+        <v>-122.2635</v>
+      </c>
+      <c r="D337" s="6" t="s">
+        <v>636</v>
+      </c>
+    </row>
+    <row r="338">
+      <c r="A338" s="6" t="s">
+        <v>637</v>
+      </c>
+      <c r="B338">
+        <f t="shared" si="2"/>
+        <v>37.86826</v>
+      </c>
+      <c r="C338">
+        <v>-122.25311</v>
+      </c>
+      <c r="D338" s="7" t="s">
+        <v>638</v>
+      </c>
+    </row>
+    <row r="339">
+      <c r="A339" s="6" t="s">
+        <v>639</v>
+      </c>
+      <c r="B339">
+        <f t="shared" si="2"/>
+        <v>37.86875</v>
+      </c>
+      <c r="C339">
+        <v>-122.26012</v>
+      </c>
+      <c r="D339" s="7" t="s">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="340">
+      <c r="A340" s="6" t="s">
+        <v>641</v>
+      </c>
+      <c r="B340">
+        <f t="shared" si="2"/>
+        <v>37.86938</v>
+      </c>
+      <c r="C340">
+        <v>-122.25928</v>
+      </c>
+      <c r="D340" s="6" t="s">
+        <v>642</v>
+      </c>
+    </row>
+    <row r="341">
+      <c r="A341" s="6" t="s">
+        <v>643</v>
+      </c>
+      <c r="B341">
+        <f t="shared" si="2"/>
+        <v>37.86782</v>
+      </c>
+      <c r="C341">
+        <v>-122.25876</v>
+      </c>
+      <c r="D341" s="7" t="s">
+        <v>644</v>
+      </c>
+    </row>
+    <row r="342">
+      <c r="A342" s="6" t="s">
+        <v>645</v>
+      </c>
+      <c r="B342">
+        <f t="shared" si="2"/>
+        <v>37.86306</v>
+      </c>
+      <c r="C342">
+        <v>-122.2578</v>
+      </c>
+      <c r="D342" s="7" t="s">
+        <v>646</v>
+      </c>
+    </row>
+    <row r="343">
+      <c r="A343" s="6" t="s">
+        <v>647</v>
+      </c>
+      <c r="B343">
+        <f t="shared" si="2"/>
+        <v>37.87147</v>
+      </c>
+      <c r="C343">
+        <v>-122.26466</v>
+      </c>
+      <c r="D343" s="7" t="s">
+        <v>648</v>
+      </c>
+    </row>
+    <row r="344">
+      <c r="A344" s="6" t="s">
+        <v>649</v>
+      </c>
+      <c r="B344">
+        <f t="shared" si="2"/>
+        <v>37.8747</v>
+      </c>
+      <c r="C344">
+        <v>-122.25793</v>
+      </c>
+      <c r="D344" s="6" t="s">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="345">
+      <c r="A345" s="6" t="s">
+        <v>651</v>
+      </c>
+      <c r="B345">
+        <f t="shared" si="2"/>
+        <v>37.86996</v>
+      </c>
+      <c r="C345">
+        <v>-122.26351</v>
+      </c>
+      <c r="D345" s="6" t="s">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="346">
+      <c r="A346" s="6" t="s">
+        <v>653</v>
+      </c>
+      <c r="B346">
+        <f t="shared" si="2"/>
+        <v>37.86476</v>
+      </c>
+      <c r="C346">
+        <v>-122.26184</v>
+      </c>
+      <c r="D346" s="8" t="s">
+        <v>654</v>
+      </c>
+    </row>
+    <row r="347">
+      <c r="A347" s="6" t="s">
+        <v>655</v>
+      </c>
+      <c r="B347">
+        <f t="shared" si="2"/>
+        <v>37.86922</v>
+      </c>
+      <c r="C347">
+        <v>-122.26321</v>
+      </c>
+      <c r="D347" s="7" t="s">
+        <v>656</v>
+      </c>
+    </row>
+    <row r="348">
+      <c r="A348" s="6" t="s">
+        <v>657</v>
+      </c>
+      <c r="B348">
+        <f t="shared" si="2"/>
+        <v>37.86655</v>
+      </c>
+      <c r="C348">
+        <v>-122.2585</v>
+      </c>
+      <c r="D348" s="7" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="349">
+      <c r="A349" s="6" t="s">
+        <v>659</v>
+      </c>
+      <c r="B349">
+        <f t="shared" si="2"/>
+        <v>37.86841</v>
+      </c>
+      <c r="C349">
+        <v>-122.25249</v>
+      </c>
+      <c r="D349" s="6" t="s">
+        <v>660</v>
+      </c>
+    </row>
+    <row r="350">
+      <c r="A350" s="6" t="s">
+        <v>661</v>
+      </c>
+      <c r="B350">
+        <f t="shared" si="2"/>
+        <v>37.86967</v>
+      </c>
+      <c r="C350">
+        <v>-122.268</v>
+      </c>
+      <c r="D350" s="7" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="351">
+      <c r="A351" s="6" t="s">
+        <v>663</v>
+      </c>
+      <c r="B351">
+        <f t="shared" si="2"/>
+        <v>37.86903</v>
+      </c>
+      <c r="C351">
+        <v>-122.25505</v>
+      </c>
+      <c r="D351" s="7" t="s">
+        <v>664</v>
+      </c>
+    </row>
+    <row r="352">
+      <c r="A352" s="6" t="s">
+        <v>665</v>
+      </c>
+      <c r="B352">
+        <f t="shared" si="2"/>
+        <v>37.86899</v>
+      </c>
+      <c r="C352">
+        <v>-122.26474</v>
+      </c>
+      <c r="D352" s="7" t="s">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="353">
+      <c r="A353" s="6" t="s">
+        <v>667</v>
+      </c>
+      <c r="B353">
+        <f t="shared" si="2"/>
+        <v>37.87505</v>
+      </c>
+      <c r="C353">
+        <v>-122.26753</v>
+      </c>
+      <c r="D353" s="6" t="s">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="354">
+      <c r="A354" s="6" t="s">
+        <v>669</v>
+      </c>
+      <c r="B354">
+        <f t="shared" si="2"/>
+        <v>37.86896</v>
+      </c>
+      <c r="C354">
+        <v>-122.2562</v>
+      </c>
+      <c r="D354" s="7" t="s">
+        <v>670</v>
+      </c>
+    </row>
+    <row r="355">
+      <c r="A355" s="6" t="s">
+        <v>671</v>
+      </c>
+      <c r="B355">
+        <f t="shared" si="2"/>
+        <v>37.87213</v>
+      </c>
+      <c r="C355">
+        <v>-122.25882</v>
+      </c>
+      <c r="D355" s="7" t="s">
+        <v>672</v>
+      </c>
+    </row>
+    <row r="356">
+      <c r="A356" s="6" t="s">
+        <v>673</v>
+      </c>
+      <c r="B356">
+        <f t="shared" si="2"/>
+        <v>37.872</v>
+      </c>
+      <c r="C356">
+        <v>-122.25751</v>
+      </c>
+      <c r="D356" s="8" t="s">
+        <v>674</v>
+      </c>
+    </row>
+    <row r="357">
+      <c r="A357" s="6" t="s">
+        <v>675</v>
+      </c>
+      <c r="B357">
+        <f t="shared" si="2"/>
+        <v>37.86821</v>
+      </c>
+      <c r="C357">
+        <v>-122.25936</v>
+      </c>
+      <c r="D357" s="6" t="s">
+        <v>676</v>
+      </c>
+    </row>
+    <row r="358">
+      <c r="A358" s="6" t="s">
+        <v>677</v>
+      </c>
+      <c r="B358">
+        <f t="shared" si="2"/>
+        <v>37.86848</v>
+      </c>
+      <c r="C358">
+        <v>-122.26352</v>
+      </c>
+      <c r="D358" s="7" t="s">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="359">
+      <c r="A359" s="6" t="s">
+        <v>679</v>
+      </c>
+      <c r="B359">
+        <f t="shared" si="2"/>
+        <v>37.86976</v>
+      </c>
+      <c r="C359">
+        <v>-122.25269</v>
+      </c>
+      <c r="D359" s="7" t="s">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="360">
+      <c r="A360" s="6" t="s">
+        <v>681</v>
+      </c>
+      <c r="B360">
+        <f t="shared" si="2"/>
+        <v>37.86591</v>
+      </c>
+      <c r="C360">
+        <v>-122.25487</v>
+      </c>
+      <c r="D360" s="7" t="s">
+        <v>682</v>
+      </c>
+    </row>
+    <row r="361">
+      <c r="A361" s="6" t="s">
+        <v>683</v>
+      </c>
+      <c r="B361">
+        <f t="shared" si="2"/>
+        <v>37.86962</v>
+      </c>
+      <c r="C361">
+        <v>-122.26061</v>
+      </c>
+      <c r="D361" s="8" t="s">
+        <v>684</v>
       </c>
     </row>
   </sheetData>

</xml_diff>